<commit_message>
Developers details and some other changes
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web development\NSS WEBSITE\NSS-Website\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51A8BBAF-965E-4034-88E7-8CAAFCC417C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A573FF-8FB2-4E0A-962B-A1360C82C627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="575">
   <si>
     <t>image</t>
   </si>
@@ -465,9 +465,6 @@
     <t>aditi43laddha@gmail.com</t>
   </si>
   <si>
-    <t>github</t>
-  </si>
-  <si>
     <t>Sushma Muppaneni</t>
   </si>
   <si>
@@ -789,12 +786,6 @@
     <t>Sudhanshu Mall</t>
   </si>
   <si>
-    <t>Neha Ma'am</t>
-  </si>
-  <si>
-    <t>Krishna Vamshi</t>
-  </si>
-  <si>
     <t>Himanshi Agarwal</t>
   </si>
   <si>
@@ -813,9 +804,6 @@
     <t>pulkitagrawal452@gmail.com</t>
   </si>
   <si>
-    <t>Vishwajeet Dwivedi</t>
-  </si>
-  <si>
     <t>Dr. Bade Mukund</t>
   </si>
   <si>
@@ -1756,6 +1744,12 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1uU7MjH2hKyV0IOg2pbwkWVzhxKmmZLDj/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sudhanshu-mall-b175b2195?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>sushilm1272@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1984,10 +1978,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2308,7 +2302,7 @@
     <col min="2" max="2" width="19.44140625" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.44140625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" style="13" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
@@ -2331,19 +2325,19 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -2394,19 +2388,19 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>244</v>
+      </c>
+      <c r="C2" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="16" t="s">
         <v>247</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2422,10 +2416,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2433,13 +2427,12 @@
     <col min="1" max="1" width="69.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.88671875" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="13"/>
+    <col min="4" max="4" width="145" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -2453,128 +2446,100 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="B2" s="23" t="s">
+        <v>253</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="28" t="s">
+        <v>436</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="D3" s="30" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C2" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D2" s="26" t="s">
+      <c r="C4" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="D4" s="30" t="s">
         <v>257</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="E4" s="29" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="13" t="s">
-        <v>255</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D3" s="23"/>
-      <c r="F3" s="23"/>
-    </row>
-    <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
-        <v>254</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28" t="s">
-        <v>440</v>
-      </c>
+    <row r="5" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="13" t="s">
         <v>252</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>233</v>
-      </c>
-      <c r="F5" s="29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
-        <v>441</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>259</v>
+        <v>428</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>573</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="28" t="s">
+        <v>438</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>248</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>260</v>
-      </c>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D7" s="23"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="28" t="s">
-        <v>442</v>
-      </c>
-      <c r="B8" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="D6" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="C8" s="19" t="s">
-        <v>432</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="E6" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="19" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
-        <v>262</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>432</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F9">
-    <sortCondition ref="B2:B9"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+    <sortCondition ref="B2:B6"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="A5" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="A6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2620,199 +2585,199 @@
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F3" s="15"/>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="E5" s="18" t="s">
         <v>238</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>239</v>
       </c>
       <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="E6" s="18" t="s">
         <v>243</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>244</v>
       </c>
       <c r="F6" s="15"/>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>233</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>234</v>
       </c>
       <c r="F7" s="15"/>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="F8" s="15"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="18" t="s">
         <v>240</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>241</v>
       </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>235</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>236</v>
       </c>
       <c r="F12" s="15"/>
     </row>
@@ -2919,667 +2884,667 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="24" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>228</v>
-      </c>
-      <c r="E2" s="19" t="s">
-        <v>229</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="E3" s="19" t="s">
         <v>195</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>196</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="E4" s="19" t="s">
         <v>161</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>162</v>
       </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>231</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>232</v>
       </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="E6" s="19" t="s">
         <v>153</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>154</v>
       </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>225</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>226</v>
       </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9" s="19" t="s">
         <v>180</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>181</v>
       </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="17" t="s">
+        <v>192</v>
+      </c>
+      <c r="E10" s="19" t="s">
         <v>193</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>194</v>
       </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="12" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>213</v>
       </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="12" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="E12" s="19" t="s">
         <v>169</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>170</v>
       </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="12" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>206</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>207</v>
       </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C14" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>186</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>187</v>
       </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="12" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C15" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>171</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>172</v>
       </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="12" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="12" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>198</v>
       </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="12" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="E18" s="19" t="s">
         <v>201</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>202</v>
       </c>
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="12" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C19" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>173</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>174</v>
       </c>
       <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="12" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="C20" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D20" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>214</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>215</v>
       </c>
       <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>219</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>220</v>
       </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>190</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>191</v>
       </c>
       <c r="F22" s="7"/>
     </row>
     <row r="23" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C23" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>204</v>
       </c>
       <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="12" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D24" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>159</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>160</v>
       </c>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="12" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="E25" s="19" t="s">
         <v>216</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>217</v>
       </c>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>156</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>157</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="12" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="E27" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E28" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>209</v>
       </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E29" s="19" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D30" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="E30" s="19" t="s">
         <v>183</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>184</v>
       </c>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="12" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="12" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="19" t="s">
         <v>151</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>152</v>
       </c>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="12" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="E33" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>176</v>
       </c>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="12" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="C34" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="E34" s="19" t="s">
         <v>199</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>200</v>
       </c>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B35" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>149</v>
       </c>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="12" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="12" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>178</v>
-      </c>
-      <c r="E37" s="13" t="s">
-        <v>179</v>
       </c>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="12" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="E38" s="13" t="s">
         <v>222</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>223</v>
       </c>
       <c r="F38" s="7"/>
     </row>
@@ -7547,8 +7512,8 @@
   </sheetPr>
   <dimension ref="A1:F1062"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7579,28 +7544,28 @@
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>5</v>
@@ -7609,16 +7574,16 @@
         <v>118</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>5</v>
@@ -7633,7 +7598,7 @@
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>13</v>
@@ -7651,7 +7616,7 @@
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>74</v>
@@ -7669,7 +7634,7 @@
     </row>
     <row r="7" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>53</v>
@@ -7678,7 +7643,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>54</v>
@@ -7687,7 +7652,7 @@
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>114</v>
@@ -7699,34 +7664,34 @@
         <v>115</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="12" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C10" s="13" t="s">
         <v>5</v>
@@ -7741,10 +7706,10 @@
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="C11" s="13" t="s">
         <v>5</v>
@@ -7759,10 +7724,10 @@
     </row>
     <row r="12" spans="1:6" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>5</v>
@@ -7777,25 +7742,25 @@
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C13" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>91</v>
@@ -7813,7 +7778,7 @@
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="B15" s="18" t="s">
         <v>19</v>
@@ -7831,10 +7796,10 @@
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C16" s="13" t="s">
         <v>5</v>
@@ -7849,7 +7814,7 @@
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="B17" s="18" t="s">
         <v>119</v>
@@ -7867,10 +7832,10 @@
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="17" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>5</v>
@@ -7885,7 +7850,7 @@
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="B19" s="18" t="s">
         <v>60</v>
@@ -7903,7 +7868,7 @@
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="B20" s="18" t="s">
         <v>24</v>
@@ -7921,34 +7886,34 @@
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F21" s="7"/>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="17" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>90</v>
@@ -7957,7 +7922,7 @@
     </row>
     <row r="23" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>94</v>
@@ -7975,7 +7940,7 @@
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>50</v>
@@ -7993,10 +7958,10 @@
     </row>
     <row r="25" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B25" s="18" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C25" s="13" t="s">
         <v>5</v>
@@ -8011,28 +7976,28 @@
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>5</v>
@@ -8047,25 +8012,25 @@
     </row>
     <row r="28" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="12" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C28" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E28" s="19" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B29" s="18" t="s">
         <v>140</v>
@@ -8083,10 +8048,10 @@
     </row>
     <row r="30" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="12" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B30" s="18" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C30" s="13" t="s">
         <v>5</v>
@@ -8101,28 +8066,28 @@
     </row>
     <row r="31" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="17" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C31" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E31" s="19" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="17" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>5</v>
@@ -8137,25 +8102,25 @@
     </row>
     <row r="33" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C33" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E33" s="19" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="17" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="B34" s="18" t="s">
         <v>129</v>
@@ -8173,10 +8138,10 @@
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>5</v>
@@ -8191,7 +8156,7 @@
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B36" s="18" t="s">
         <v>66</v>
@@ -8209,7 +8174,7 @@
     </row>
     <row r="37" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="B37" s="18" t="s">
         <v>82</v>
@@ -8227,7 +8192,7 @@
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B38" s="18" t="s">
         <v>34</v>
@@ -8245,28 +8210,28 @@
     </row>
     <row r="39" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="12" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>5</v>
@@ -8275,16 +8240,16 @@
         <v>18</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>5</v>
@@ -8299,100 +8264,100 @@
     </row>
     <row r="42" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="12" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="17" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>5</v>
@@ -8407,7 +8372,7 @@
     </row>
     <row r="48" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="12" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B48" s="18" t="s">
         <v>136</v>
@@ -8425,28 +8390,28 @@
     </row>
     <row r="49" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>5</v>
@@ -8461,10 +8426,10 @@
     </row>
     <row r="51" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>5</v>
@@ -8479,10 +8444,10 @@
     </row>
     <row r="52" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>5</v>
@@ -8497,7 +8462,7 @@
     </row>
     <row r="53" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B53" s="18" t="s">
         <v>122</v>
@@ -8515,25 +8480,25 @@
     </row>
     <row r="54" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="12" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B55" s="18" t="s">
         <v>97</v>
@@ -8551,61 +8516,61 @@
     </row>
     <row r="56" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>362</v>
+        <v>326</v>
+      </c>
+      <c r="E56" s="20" t="s">
+        <v>358</v>
       </c>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="E57" s="19" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B59" s="18" t="s">
         <v>107</v>
@@ -8623,7 +8588,7 @@
     </row>
     <row r="60" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B60" s="18" t="s">
         <v>29</v>
@@ -8641,25 +8606,25 @@
     </row>
     <row r="61" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61" s="12" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="F61" s="7"/>
     </row>
     <row r="62" spans="1:6" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="17" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="B62" s="18" t="s">
         <v>104</v>
@@ -8677,7 +8642,7 @@
     </row>
     <row r="63" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="12" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B63" s="18" t="s">
         <v>63</v>
@@ -8695,10 +8660,10 @@
     </row>
     <row r="64" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="17" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>5</v>
@@ -8713,10 +8678,10 @@
     </row>
     <row r="65" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>5</v>
@@ -8725,34 +8690,34 @@
         <v>125</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>5</v>
@@ -8767,7 +8732,7 @@
     </row>
     <row r="68" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="12" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B68" s="18" t="s">
         <v>8</v>
@@ -8785,7 +8750,7 @@
     </row>
     <row r="69" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A69" s="17" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B69" s="18" t="s">
         <v>126</v>
@@ -8796,53 +8761,53 @@
       <c r="D69" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="E69" s="13" t="s">
+      <c r="E69" s="24" t="s">
         <v>128</v>
       </c>
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="E70" s="13" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="F71" s="7"/>
     </row>
     <row r="72" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>5</v>
@@ -8857,7 +8822,7 @@
     </row>
     <row r="73" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B73" s="18" t="s">
         <v>39</v>
@@ -8875,10 +8840,10 @@
     </row>
     <row r="74" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>5</v>
@@ -8887,34 +8852,34 @@
         <v>143</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>5</v>
@@ -8923,34 +8888,34 @@
         <v>139</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F76" s="7"/>
     </row>
     <row r="77" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A77" s="12" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="F77" s="7"/>
     </row>
     <row r="78" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>5</v>
@@ -8965,10 +8930,10 @@
     </row>
     <row r="79" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>5</v>
@@ -8983,10 +8948,10 @@
     </row>
     <row r="80" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="12" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>5</v>
@@ -9001,61 +8966,61 @@
     </row>
     <row r="81" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="F81" s="7"/>
     </row>
     <row r="82" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="F82" s="7"/>
     </row>
     <row r="83" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="F83" s="7"/>
     </row>
     <row r="84" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" s="12" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="B84" s="18" t="s">
         <v>87</v>
@@ -9073,25 +9038,25 @@
     </row>
     <row r="85" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85" s="17" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="F85" s="7"/>
     </row>
     <row r="86" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="B86" s="18" t="s">
         <v>71</v>
@@ -9109,7 +9074,7 @@
     </row>
     <row r="87" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B87" s="18" t="s">
         <v>79</v>
@@ -9127,7 +9092,7 @@
     </row>
     <row r="88" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="B88" s="18" t="s">
         <v>55</v>
@@ -9145,10 +9110,10 @@
     </row>
     <row r="89" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>5</v>
@@ -13865,8 +13830,10 @@
     <hyperlink ref="A47" r:id="rId94" xr:uid="{3874B9EB-2CBF-4C6B-8F13-149322316408}"/>
     <hyperlink ref="A53" r:id="rId95" xr:uid="{725311D9-B8BF-4922-90EC-D5D8E78083DD}"/>
     <hyperlink ref="A55" r:id="rId96" xr:uid="{240F5350-5B92-451C-818B-02F6D13E3BAA}"/>
+    <hyperlink ref="E69" r:id="rId97" xr:uid="{57E52675-2220-49AA-876F-C78370CAB07B}"/>
+    <hyperlink ref="E56" r:id="rId98" xr:uid="{7BED298F-EEA1-4144-9433-7D514F1D86B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId97"/>
+  <pageSetup orientation="portrait" r:id="rId99"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
All Events added + my photo
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Github\Final NSS Website\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E47242-5F30-42A6-A47C-AE99877029BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="581">
   <si>
     <t>image</t>
   </si>
@@ -1756,12 +1755,24 @@
   </si>
   <si>
     <t>https://drive.google.com/file/d/1eu13qMDF0rJzooJ_LEcQc7xBHtylyx4Q/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1emfchxV1KCWoBRjdfr4Di8XQ1RuTo5qj/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>Harshit Pathak</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/harshit-pathak-4ba6aa22a/</t>
+  </si>
+  <si>
+    <t>pathakharshit281@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2292,7 +2303,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2348,14 +2359,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{03AB67D4-9C5B-4A72-8EA4-E313AD2CE085}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2411,14 +2422,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2541,21 +2552,21 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E6">
+  <sortState ref="A2:E6">
     <sortCondition ref="B2:B6"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
-    <hyperlink ref="A4" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A2" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2830,24 +2841,24 @@
     <row r="50" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E12">
+  <sortState ref="A2:E12">
     <sortCondition ref="B2:B12"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
-    <hyperlink ref="D10" r:id="rId8" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
-    <hyperlink ref="D11" r:id="rId9" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
-    <hyperlink ref="A2" r:id="rId11" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
-    <hyperlink ref="A4" r:id="rId12" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
-    <hyperlink ref="A5" r:id="rId13" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
-    <hyperlink ref="A3" r:id="rId14" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
+    <hyperlink ref="D5" r:id="rId3"/>
+    <hyperlink ref="D6" r:id="rId4"/>
+    <hyperlink ref="D7" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D9" r:id="rId7"/>
+    <hyperlink ref="D10" r:id="rId8"/>
+    <hyperlink ref="D11" r:id="rId9"/>
+    <hyperlink ref="D12" r:id="rId10"/>
+    <hyperlink ref="A2" r:id="rId11"/>
+    <hyperlink ref="A4" r:id="rId12"/>
+    <hyperlink ref="A5" r:id="rId13"/>
+    <hyperlink ref="A3" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
@@ -2855,7 +2866,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -7459,70 +7470,70 @@
       <c r="D1040" s="4"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E38">
+  <sortState ref="A2:E38">
     <sortCondition ref="B2:B38"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" display="http://www.linkedin.com/in/hemanth-kumar-avidi-814b93226" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
-    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
-    <hyperlink ref="D11" r:id="rId10" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
-    <hyperlink ref="D12" r:id="rId11" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
-    <hyperlink ref="D13" r:id="rId12" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
-    <hyperlink ref="D14" r:id="rId13" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
-    <hyperlink ref="D16" r:id="rId15" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
-    <hyperlink ref="D17" r:id="rId16" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
-    <hyperlink ref="D18" r:id="rId17" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
-    <hyperlink ref="D19" r:id="rId18" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
-    <hyperlink ref="D20" r:id="rId19" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
-    <hyperlink ref="D21" r:id="rId20" display="http://www.linkedin.com/in/krupa-vaghamshi" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
-    <hyperlink ref="D22" r:id="rId21" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
-    <hyperlink ref="D23" r:id="rId22" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
-    <hyperlink ref="D24" r:id="rId23" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
-    <hyperlink ref="D25" r:id="rId24" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
-    <hyperlink ref="D26" r:id="rId25" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
-    <hyperlink ref="D27" r:id="rId26" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
-    <hyperlink ref="D28" r:id="rId27" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
-    <hyperlink ref="D29" r:id="rId28" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
-    <hyperlink ref="D30" r:id="rId29" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
-    <hyperlink ref="D34" r:id="rId33" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
-    <hyperlink ref="D35" r:id="rId34" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
-    <hyperlink ref="D36" r:id="rId35" display="http://www.linkedin.com/in/teena413" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
-    <hyperlink ref="D37" r:id="rId36" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
-    <hyperlink ref="D38" r:id="rId37" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
-    <hyperlink ref="A5" r:id="rId38" xr:uid="{BE6C5CE3-C6AF-4FCA-8392-D259AE560322}"/>
-    <hyperlink ref="A32" r:id="rId39" xr:uid="{D8CAA88D-8EE7-4468-84DA-2C4C27314758}"/>
-    <hyperlink ref="A2" r:id="rId40" xr:uid="{73380BB2-3DB6-4F3D-9419-56E747492E63}"/>
-    <hyperlink ref="A3" r:id="rId41" xr:uid="{9A2F0BFA-B182-497A-A07D-076B6D799F4F}"/>
-    <hyperlink ref="A4" r:id="rId42" xr:uid="{4689E078-2E87-4167-8029-47337C2EBC9A}"/>
-    <hyperlink ref="A6" r:id="rId43" xr:uid="{DAECBF89-81B8-4753-AB8B-645935AEB7AA}"/>
-    <hyperlink ref="A7" r:id="rId44" xr:uid="{FC2C7287-A0F9-4CA2-8DE6-194FE7FC8990}"/>
-    <hyperlink ref="A11" r:id="rId45" xr:uid="{4BB9B0BB-5752-4199-9B23-FA554AD2F1CD}"/>
-    <hyperlink ref="A9" r:id="rId46" xr:uid="{B38BB176-A08C-4410-8602-E49161FBDB1A}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5" display="http://www.linkedin.com/in/hemanth-kumar-avidi-814b93226"/>
+    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D8" r:id="rId7"/>
+    <hyperlink ref="D9" r:id="rId8"/>
+    <hyperlink ref="D10" r:id="rId9"/>
+    <hyperlink ref="D11" r:id="rId10"/>
+    <hyperlink ref="D12" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId12"/>
+    <hyperlink ref="D14" r:id="rId13"/>
+    <hyperlink ref="D15" r:id="rId14"/>
+    <hyperlink ref="D16" r:id="rId15"/>
+    <hyperlink ref="D17" r:id="rId16"/>
+    <hyperlink ref="D18" r:id="rId17"/>
+    <hyperlink ref="D19" r:id="rId18"/>
+    <hyperlink ref="D20" r:id="rId19"/>
+    <hyperlink ref="D21" r:id="rId20" display="http://www.linkedin.com/in/krupa-vaghamshi"/>
+    <hyperlink ref="D22" r:id="rId21"/>
+    <hyperlink ref="D23" r:id="rId22"/>
+    <hyperlink ref="D24" r:id="rId23"/>
+    <hyperlink ref="D25" r:id="rId24"/>
+    <hyperlink ref="D26" r:id="rId25"/>
+    <hyperlink ref="D27" r:id="rId26"/>
+    <hyperlink ref="D28" r:id="rId27"/>
+    <hyperlink ref="D29" r:id="rId28"/>
+    <hyperlink ref="D30" r:id="rId29"/>
+    <hyperlink ref="D31" r:id="rId30"/>
+    <hyperlink ref="D32" r:id="rId31"/>
+    <hyperlink ref="D33" r:id="rId32"/>
+    <hyperlink ref="D34" r:id="rId33"/>
+    <hyperlink ref="D35" r:id="rId34"/>
+    <hyperlink ref="D36" r:id="rId35" display="http://www.linkedin.com/in/teena413"/>
+    <hyperlink ref="D37" r:id="rId36"/>
+    <hyperlink ref="D38" r:id="rId37"/>
+    <hyperlink ref="A5" r:id="rId38"/>
+    <hyperlink ref="A32" r:id="rId39"/>
+    <hyperlink ref="A2" r:id="rId40"/>
+    <hyperlink ref="A3" r:id="rId41"/>
+    <hyperlink ref="A4" r:id="rId42"/>
+    <hyperlink ref="A6" r:id="rId43"/>
+    <hyperlink ref="A7" r:id="rId44"/>
+    <hyperlink ref="A11" r:id="rId45"/>
+    <hyperlink ref="A9" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F1062"/>
+  <dimension ref="A1:F1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="62" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A125" zoomScale="91" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8147,1003 +8158,1020 @@
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="17" t="s">
-        <v>518</v>
+        <v>577</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>278</v>
+        <v>578</v>
       </c>
       <c r="C35" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>12</v>
+        <v>579</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>580</v>
       </c>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="17" t="s">
-        <v>552</v>
+        <v>518</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>66</v>
+        <v>278</v>
       </c>
       <c r="C36" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>67</v>
+        <v>11</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>517</v>
+        <v>552</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="C37" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="E37" s="19" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F37" s="7"/>
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>553</v>
+        <v>517</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="17" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="F38" s="7"/>
     </row>
     <row r="39" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
-        <v>515</v>
+        <v>553</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>279</v>
+        <v>34</v>
       </c>
       <c r="C39" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>318</v>
+        <v>35</v>
       </c>
       <c r="E39" s="19" t="s">
-        <v>349</v>
+        <v>36</v>
       </c>
       <c r="F39" s="7"/>
     </row>
     <row r="40" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="12" t="s">
-        <v>514</v>
+      <c r="A40" s="17" t="s">
+        <v>515</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>18</v>
+        <v>318</v>
       </c>
       <c r="E40" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F40" s="7"/>
     </row>
     <row r="41" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="12" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C41" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="17" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="E41" s="19" t="s">
-        <v>47</v>
+        <v>350</v>
       </c>
       <c r="F41" s="7"/>
     </row>
     <row r="42" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="12" t="s">
-        <v>554</v>
+        <v>513</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>422</v>
+        <v>281</v>
       </c>
       <c r="C42" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>319</v>
+        <v>46</v>
       </c>
       <c r="E42" s="19" t="s">
-        <v>351</v>
+        <v>47</v>
       </c>
       <c r="F42" s="7"/>
     </row>
     <row r="43" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="17" t="s">
-        <v>512</v>
+      <c r="A43" s="12" t="s">
+        <v>554</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>282</v>
+        <v>422</v>
       </c>
       <c r="C43" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E43" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F43" s="7"/>
     </row>
     <row r="44" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="12" t="s">
-        <v>509</v>
+      <c r="A44" s="17" t="s">
+        <v>512</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C44" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E44" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F44" s="7"/>
     </row>
     <row r="45" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="12" t="s">
-        <v>555</v>
+        <v>509</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C45" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D45" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E45" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F45" s="7"/>
     </row>
     <row r="46" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
-        <v>533</v>
+      <c r="A46" s="12" t="s">
+        <v>555</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C46" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E46" s="19" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F46" s="7"/>
     </row>
     <row r="47" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="17" t="s">
-        <v>556</v>
+        <v>533</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>85</v>
+        <v>323</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>86</v>
+        <v>355</v>
       </c>
       <c r="F47" s="7"/>
     </row>
     <row r="48" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12" t="s">
-        <v>557</v>
+      <c r="A48" s="17" t="s">
+        <v>556</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>136</v>
+        <v>286</v>
       </c>
       <c r="C48" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>137</v>
+        <v>85</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>138</v>
+        <v>86</v>
       </c>
       <c r="F48" s="7"/>
     </row>
     <row r="49" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="17" t="s">
-        <v>558</v>
+      <c r="A49" s="12" t="s">
+        <v>557</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>287</v>
+        <v>136</v>
       </c>
       <c r="C49" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>324</v>
+        <v>137</v>
       </c>
       <c r="E49" s="19" t="s">
-        <v>356</v>
+        <v>138</v>
       </c>
       <c r="F49" s="7"/>
     </row>
     <row r="50" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="17" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>419</v>
+        <v>287</v>
       </c>
       <c r="C50" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>48</v>
+        <v>324</v>
       </c>
       <c r="E50" s="19" t="s">
-        <v>49</v>
+        <v>356</v>
       </c>
       <c r="F50" s="7"/>
     </row>
     <row r="51" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="B51" s="18" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="C51" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>116</v>
+        <v>48</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
       <c r="F51" s="7"/>
     </row>
     <row r="52" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="12" t="s">
-        <v>567</v>
+      <c r="A52" s="17" t="s">
+        <v>560</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>288</v>
+        <v>423</v>
       </c>
       <c r="C52" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>42</v>
+        <v>116</v>
       </c>
       <c r="E52" s="19" t="s">
-        <v>43</v>
+        <v>117</v>
       </c>
       <c r="F52" s="7"/>
     </row>
     <row r="53" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="17" t="s">
-        <v>561</v>
+      <c r="A53" s="12" t="s">
+        <v>567</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>122</v>
+        <v>288</v>
       </c>
       <c r="C53" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="E53" s="19" t="s">
-        <v>124</v>
+        <v>43</v>
       </c>
       <c r="F53" s="7"/>
     </row>
     <row r="54" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="12" t="s">
-        <v>565</v>
+      <c r="A54" s="17" t="s">
+        <v>561</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>424</v>
+        <v>122</v>
       </c>
       <c r="C54" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>325</v>
+        <v>123</v>
       </c>
       <c r="E54" s="19" t="s">
-        <v>357</v>
+        <v>124</v>
       </c>
       <c r="F54" s="7"/>
     </row>
     <row r="55" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="12" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="B55" s="18" t="s">
-        <v>97</v>
+        <v>424</v>
       </c>
       <c r="C55" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>98</v>
+        <v>325</v>
       </c>
       <c r="E55" s="19" t="s">
-        <v>99</v>
+        <v>357</v>
       </c>
       <c r="F55" s="7"/>
     </row>
     <row r="56" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="12" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>289</v>
+        <v>97</v>
       </c>
       <c r="C56" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="E56" s="20" t="s">
-        <v>358</v>
+        <v>98</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="F56" s="7"/>
     </row>
     <row r="57" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57" s="17" t="s">
-        <v>574</v>
+      <c r="A57" s="12" t="s">
+        <v>563</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C57" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>359</v>
+        <v>326</v>
+      </c>
+      <c r="E57" s="20" t="s">
+        <v>358</v>
       </c>
       <c r="F57" s="7"/>
     </row>
     <row r="58" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>549</v>
+        <v>574</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>420</v>
+        <v>290</v>
       </c>
       <c r="C58" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E58" s="19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="F58" s="7"/>
     </row>
     <row r="59" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
-        <v>564</v>
+        <v>549</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>107</v>
+        <v>420</v>
       </c>
       <c r="C59" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>108</v>
+        <v>328</v>
       </c>
       <c r="E59" s="19" t="s">
-        <v>109</v>
+        <v>360</v>
       </c>
       <c r="F59" s="7"/>
     </row>
     <row r="60" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
-        <v>543</v>
+        <v>564</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>29</v>
+        <v>107</v>
       </c>
       <c r="C60" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>30</v>
+        <v>108</v>
       </c>
       <c r="E60" s="19" t="s">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="F60" s="7"/>
     </row>
     <row r="61" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="12" t="s">
-        <v>542</v>
+      <c r="A61" s="17" t="s">
+        <v>543</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>291</v>
+        <v>29</v>
       </c>
       <c r="C61" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>329</v>
+        <v>30</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>361</v>
+        <v>31</v>
       </c>
       <c r="F61" s="7"/>
     </row>
-    <row r="62" spans="1:6" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="17" t="s">
-        <v>544</v>
+    <row r="62" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="12" t="s">
+        <v>542</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>104</v>
+        <v>291</v>
       </c>
       <c r="C62" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D62" s="17" t="s">
-        <v>105</v>
+        <v>329</v>
       </c>
       <c r="E62" s="19" t="s">
-        <v>106</v>
+        <v>361</v>
       </c>
       <c r="F62" s="7"/>
     </row>
-    <row r="63" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="12" t="s">
-        <v>545</v>
+    <row r="63" spans="1:6" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="17" t="s">
+        <v>544</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>63</v>
+        <v>104</v>
       </c>
       <c r="C63" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>64</v>
+        <v>105</v>
       </c>
       <c r="E63" s="19" t="s">
-        <v>65</v>
+        <v>106</v>
       </c>
       <c r="F63" s="7"/>
     </row>
     <row r="64" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="17" t="s">
-        <v>546</v>
+      <c r="A64" s="12" t="s">
+        <v>545</v>
       </c>
       <c r="B64" s="18" t="s">
-        <v>292</v>
+        <v>63</v>
       </c>
       <c r="C64" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D64" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" s="13" t="s">
-        <v>101</v>
+        <v>64</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>65</v>
       </c>
       <c r="F64" s="7"/>
     </row>
     <row r="65" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="17" t="s">
-        <v>532</v>
+        <v>546</v>
       </c>
       <c r="B65" s="18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C65" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="E65" s="13" t="s">
-        <v>362</v>
+        <v>101</v>
       </c>
       <c r="F65" s="7"/>
     </row>
     <row r="66" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="17" t="s">
-        <v>547</v>
+        <v>532</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C66" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D66" s="17" t="s">
-        <v>330</v>
+        <v>125</v>
       </c>
       <c r="E66" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="F66" s="7"/>
     </row>
     <row r="67" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="17" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B67" s="18" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C67" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>27</v>
+        <v>330</v>
       </c>
       <c r="E67" s="13" t="s">
-        <v>28</v>
+        <v>363</v>
       </c>
       <c r="F67" s="7"/>
     </row>
     <row r="68" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="12" t="s">
-        <v>550</v>
+      <c r="A68" s="17" t="s">
+        <v>548</v>
       </c>
       <c r="B68" s="18" t="s">
-        <v>8</v>
+        <v>295</v>
       </c>
       <c r="C68" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="E68" s="13" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F68" s="7"/>
     </row>
     <row r="69" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="17" t="s">
-        <v>551</v>
+      <c r="A69" s="12" t="s">
+        <v>550</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>126</v>
+        <v>8</v>
       </c>
       <c r="C69" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="E69" s="24" t="s">
-        <v>128</v>
+        <v>9</v>
+      </c>
+      <c r="E69" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="F69" s="7"/>
     </row>
     <row r="70" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="17" t="s">
-        <v>566</v>
+        <v>551</v>
       </c>
       <c r="B70" s="18" t="s">
-        <v>296</v>
+        <v>126</v>
       </c>
       <c r="C70" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>331</v>
-      </c>
-      <c r="E70" s="13" t="s">
-        <v>364</v>
+        <v>127</v>
+      </c>
+      <c r="E70" s="24" t="s">
+        <v>128</v>
       </c>
       <c r="F70" s="7"/>
     </row>
     <row r="71" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="17" t="s">
-        <v>576</v>
+        <v>566</v>
       </c>
       <c r="B71" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C71" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E71" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F71" s="7"/>
     </row>
     <row r="72" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="17" t="s">
-        <v>568</v>
+        <v>576</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C72" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D72" s="17" t="s">
-        <v>132</v>
+        <v>332</v>
       </c>
       <c r="E72" s="13" t="s">
-        <v>133</v>
+        <v>365</v>
       </c>
       <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>39</v>
+        <v>298</v>
       </c>
       <c r="C73" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>40</v>
+        <v>132</v>
       </c>
       <c r="E73" s="13" t="s">
-        <v>41</v>
+        <v>133</v>
       </c>
       <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A74" s="17" t="s">
-        <v>511</v>
+        <v>569</v>
       </c>
       <c r="B74" s="18" t="s">
-        <v>299</v>
+        <v>39</v>
       </c>
       <c r="C74" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="E74" s="13" t="s">
-        <v>366</v>
+        <v>41</v>
       </c>
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="17" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C75" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>333</v>
+        <v>143</v>
       </c>
       <c r="E75" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A76" s="17" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="B76" s="18" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C76" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>139</v>
+        <v>333</v>
       </c>
       <c r="E76" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="F76" s="7"/>
     </row>
     <row r="77" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="12" t="s">
-        <v>571</v>
+      <c r="A77" s="17" t="s">
+        <v>508</v>
       </c>
       <c r="B77" s="18" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C77" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D77" s="17" t="s">
-        <v>334</v>
+        <v>139</v>
       </c>
       <c r="E77" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="F77" s="7"/>
     </row>
     <row r="78" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="17" t="s">
-        <v>507</v>
+      <c r="A78" s="12" t="s">
+        <v>571</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>425</v>
+        <v>302</v>
       </c>
       <c r="C78" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D78" s="17" t="s">
-        <v>58</v>
+        <v>334</v>
       </c>
       <c r="E78" s="13" t="s">
-        <v>59</v>
+        <v>369</v>
       </c>
       <c r="F78" s="7"/>
     </row>
     <row r="79" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B79" s="18" t="s">
-        <v>303</v>
+        <v>425</v>
       </c>
       <c r="C79" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="17" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="E79" s="13" t="s">
-        <v>33</v>
+        <v>59</v>
       </c>
       <c r="F79" s="7"/>
     </row>
     <row r="80" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="12" t="s">
-        <v>505</v>
+      <c r="A80" s="17" t="s">
+        <v>506</v>
       </c>
       <c r="B80" s="18" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C80" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D80" s="17" t="s">
-        <v>112</v>
+        <v>32</v>
       </c>
       <c r="E80" s="13" t="s">
-        <v>113</v>
+        <v>33</v>
       </c>
       <c r="F80" s="7"/>
     </row>
     <row r="81" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A81" s="17" t="s">
-        <v>504</v>
+      <c r="A81" s="12" t="s">
+        <v>505</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C81" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>335</v>
+        <v>112</v>
       </c>
       <c r="E81" s="13" t="s">
-        <v>370</v>
+        <v>113</v>
       </c>
       <c r="F81" s="7"/>
     </row>
     <row r="82" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B82" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C82" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D82" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E82" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F82" s="7"/>
     </row>
     <row r="83" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="B83" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C83" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D83" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E83" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="F83" s="7"/>
     </row>
     <row r="84" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A84" s="12" t="s">
-        <v>501</v>
+      <c r="A84" s="17" t="s">
+        <v>502</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>87</v>
+        <v>307</v>
       </c>
       <c r="C84" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D84" s="17" t="s">
-        <v>88</v>
+        <v>337</v>
       </c>
       <c r="E84" s="13" t="s">
-        <v>89</v>
+        <v>372</v>
       </c>
       <c r="F84" s="7"/>
     </row>
     <row r="85" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="17" t="s">
-        <v>500</v>
+      <c r="A85" s="12" t="s">
+        <v>501</v>
       </c>
       <c r="B85" s="18" t="s">
-        <v>308</v>
+        <v>87</v>
       </c>
       <c r="C85" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>338</v>
+        <v>88</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>373</v>
+        <v>89</v>
       </c>
       <c r="F85" s="7"/>
     </row>
     <row r="86" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" s="17" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>71</v>
+        <v>308</v>
       </c>
       <c r="C86" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D86" s="17" t="s">
-        <v>72</v>
+        <v>338</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>73</v>
+        <v>373</v>
       </c>
       <c r="F86" s="7"/>
     </row>
     <row r="87" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A87" s="17" t="s">
-        <v>516</v>
+        <v>499</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C87" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D87" s="17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="F87" s="7"/>
     </row>
     <row r="88" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" s="17" t="s">
-        <v>498</v>
+        <v>516</v>
       </c>
       <c r="B88" s="18" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="C88" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D88" s="17" t="s">
-        <v>56</v>
+        <v>80</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="F88" s="7"/>
     </row>
     <row r="89" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89" s="17" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="B89" s="18" t="s">
-        <v>309</v>
+        <v>55</v>
       </c>
       <c r="C89" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D89" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F89" s="7"/>
+    </row>
+    <row r="90" spans="1:6" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A90" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="B90" s="18" t="s">
+        <v>309</v>
+      </c>
+      <c r="C90" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D90" s="17" t="s">
         <v>102</v>
       </c>
-      <c r="E89" s="13" t="s">
+      <c r="E90" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="F89" s="7"/>
-    </row>
-    <row r="90" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="7"/>
-      <c r="B90" s="8"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="7"/>
-      <c r="E90" s="8"/>
       <c r="F90" s="7"/>
     </row>
-    <row r="91" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="7"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="7"/>
+    </row>
     <row r="92" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="93" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -9177,12 +9205,8 @@
     <row r="122" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="123" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="124" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="151" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A151" s="4"/>
-      <c r="B151" s="4"/>
-      <c r="D151" s="5"/>
-    </row>
+    <row r="125" ht="19.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="151" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="152" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A152" s="4"/>
       <c r="B152" s="4"/>
@@ -13738,113 +13762,121 @@
       <c r="B1062" s="4"/>
       <c r="D1062" s="5"/>
     </row>
+    <row r="1063" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1063" s="4"/>
+      <c r="B1063" s="4"/>
+      <c r="D1063" s="5"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E89">
+  <sortState ref="A2:E89">
     <sortCondition ref="B2:B89"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000058000000}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000059000000}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0500-00005A000000}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{00000000-0004-0000-0500-00005B000000}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{00000000-0004-0000-0500-00005C000000}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{00000000-0004-0000-0500-00005D000000}"/>
-    <hyperlink ref="D10" r:id="rId7" xr:uid="{00000000-0004-0000-0500-00005E000000}"/>
-    <hyperlink ref="D11" r:id="rId8" xr:uid="{00000000-0004-0000-0500-00005F000000}"/>
-    <hyperlink ref="D12" r:id="rId9" xr:uid="{00000000-0004-0000-0500-000060000000}"/>
-    <hyperlink ref="D13" r:id="rId10" xr:uid="{00000000-0004-0000-0500-000061000000}"/>
-    <hyperlink ref="D14" r:id="rId11" xr:uid="{00000000-0004-0000-0500-000062000000}"/>
-    <hyperlink ref="D15" r:id="rId12" display="http://www.linkedin.com/in/anushkjoshi" xr:uid="{00000000-0004-0000-0500-000063000000}"/>
-    <hyperlink ref="D16" r:id="rId13" xr:uid="{00000000-0004-0000-0500-000064000000}"/>
-    <hyperlink ref="D17" r:id="rId14" xr:uid="{00000000-0004-0000-0500-000065000000}"/>
-    <hyperlink ref="D18" r:id="rId15" xr:uid="{00000000-0004-0000-0500-000066000000}"/>
-    <hyperlink ref="D19" r:id="rId16" display="http://linkedin.com/in/arjama-mohanty-17616a243" xr:uid="{00000000-0004-0000-0500-000067000000}"/>
-    <hyperlink ref="D20" r:id="rId17" xr:uid="{00000000-0004-0000-0500-000068000000}"/>
-    <hyperlink ref="D21" r:id="rId18" xr:uid="{00000000-0004-0000-0500-000069000000}"/>
-    <hyperlink ref="D23" r:id="rId19" xr:uid="{00000000-0004-0000-0500-00006A000000}"/>
-    <hyperlink ref="D24" r:id="rId20" xr:uid="{00000000-0004-0000-0500-00006B000000}"/>
-    <hyperlink ref="D25" r:id="rId21" xr:uid="{00000000-0004-0000-0500-00006C000000}"/>
-    <hyperlink ref="D26" r:id="rId22" xr:uid="{00000000-0004-0000-0500-00006D000000}"/>
-    <hyperlink ref="D27" r:id="rId23" xr:uid="{00000000-0004-0000-0500-00006E000000}"/>
-    <hyperlink ref="D28" r:id="rId24" xr:uid="{00000000-0004-0000-0500-00006F000000}"/>
-    <hyperlink ref="D29" r:id="rId25" xr:uid="{00000000-0004-0000-0500-000070000000}"/>
-    <hyperlink ref="D30" r:id="rId26" xr:uid="{00000000-0004-0000-0500-000071000000}"/>
-    <hyperlink ref="D31" r:id="rId27" xr:uid="{00000000-0004-0000-0500-000072000000}"/>
-    <hyperlink ref="D32" r:id="rId28" xr:uid="{00000000-0004-0000-0500-000073000000}"/>
-    <hyperlink ref="D33" r:id="rId29" display="http://www.linkedin.com/in/priya-gadariya-a21312248" xr:uid="{00000000-0004-0000-0500-000074000000}"/>
-    <hyperlink ref="D34" r:id="rId30" xr:uid="{00000000-0004-0000-0500-000075000000}"/>
-    <hyperlink ref="D35" r:id="rId31" xr:uid="{00000000-0004-0000-0500-000076000000}"/>
-    <hyperlink ref="D36" r:id="rId32" xr:uid="{00000000-0004-0000-0500-000077000000}"/>
-    <hyperlink ref="D37" r:id="rId33" xr:uid="{00000000-0004-0000-0500-000078000000}"/>
-    <hyperlink ref="D38" r:id="rId34" display="http://linkedin.com/in/jinhal-maheshwari-71a217212/" xr:uid="{00000000-0004-0000-0500-000079000000}"/>
-    <hyperlink ref="D39" r:id="rId35" xr:uid="{00000000-0004-0000-0500-00007A000000}"/>
-    <hyperlink ref="D40" r:id="rId36" xr:uid="{00000000-0004-0000-0500-00007B000000}"/>
-    <hyperlink ref="D41" r:id="rId37" display="http://linkedin.in/in/kevalkanpariya" xr:uid="{00000000-0004-0000-0500-00007C000000}"/>
-    <hyperlink ref="D42" r:id="rId38" xr:uid="{00000000-0004-0000-0500-00007D000000}"/>
-    <hyperlink ref="D43" r:id="rId39" xr:uid="{00000000-0004-0000-0500-00007E000000}"/>
-    <hyperlink ref="D44" r:id="rId40" xr:uid="{00000000-0004-0000-0500-00007F000000}"/>
-    <hyperlink ref="D45" r:id="rId41" xr:uid="{00000000-0004-0000-0500-000080000000}"/>
-    <hyperlink ref="D46" r:id="rId42" xr:uid="{00000000-0004-0000-0500-000081000000}"/>
-    <hyperlink ref="D47" r:id="rId43" xr:uid="{00000000-0004-0000-0500-000082000000}"/>
-    <hyperlink ref="D48" r:id="rId44" xr:uid="{00000000-0004-0000-0500-000083000000}"/>
-    <hyperlink ref="D49" r:id="rId45" xr:uid="{00000000-0004-0000-0500-000084000000}"/>
-    <hyperlink ref="D50" r:id="rId46" xr:uid="{00000000-0004-0000-0500-000085000000}"/>
-    <hyperlink ref="D51" r:id="rId47" xr:uid="{00000000-0004-0000-0500-000086000000}"/>
-    <hyperlink ref="D52" r:id="rId48" xr:uid="{00000000-0004-0000-0500-000087000000}"/>
-    <hyperlink ref="D53" r:id="rId49" display="http://www.linkedin.com/in/nishank-sudhir-654924228" xr:uid="{00000000-0004-0000-0500-000088000000}"/>
-    <hyperlink ref="D54" r:id="rId50" xr:uid="{00000000-0004-0000-0500-000089000000}"/>
-    <hyperlink ref="D55" r:id="rId51" xr:uid="{00000000-0004-0000-0500-00008A000000}"/>
-    <hyperlink ref="D56" r:id="rId52" display="https://in.linkedin.com/in/pragnesh-barik" xr:uid="{00000000-0004-0000-0500-00008B000000}"/>
-    <hyperlink ref="D57" r:id="rId53" xr:uid="{00000000-0004-0000-0500-00008C000000}"/>
-    <hyperlink ref="D58" r:id="rId54" display="https://pranitsatpute.com/" xr:uid="{00000000-0004-0000-0500-00008D000000}"/>
-    <hyperlink ref="D59" r:id="rId55" xr:uid="{00000000-0004-0000-0500-00008E000000}"/>
-    <hyperlink ref="D60" r:id="rId56" xr:uid="{00000000-0004-0000-0500-00008F000000}"/>
-    <hyperlink ref="D61" r:id="rId57" xr:uid="{00000000-0004-0000-0500-000090000000}"/>
-    <hyperlink ref="D62" r:id="rId58" xr:uid="{00000000-0004-0000-0500-000091000000}"/>
-    <hyperlink ref="D63" r:id="rId59" xr:uid="{00000000-0004-0000-0500-000092000000}"/>
-    <hyperlink ref="D64" r:id="rId60" xr:uid="{00000000-0004-0000-0500-000093000000}"/>
-    <hyperlink ref="D65" r:id="rId61" xr:uid="{00000000-0004-0000-0500-000094000000}"/>
-    <hyperlink ref="D66" r:id="rId62" xr:uid="{00000000-0004-0000-0500-000095000000}"/>
-    <hyperlink ref="D67" r:id="rId63" xr:uid="{00000000-0004-0000-0500-000096000000}"/>
-    <hyperlink ref="D68" r:id="rId64" xr:uid="{00000000-0004-0000-0500-000097000000}"/>
-    <hyperlink ref="D69" r:id="rId65" xr:uid="{00000000-0004-0000-0500-000098000000}"/>
-    <hyperlink ref="D70" r:id="rId66" xr:uid="{00000000-0004-0000-0500-000099000000}"/>
-    <hyperlink ref="D71" r:id="rId67" xr:uid="{00000000-0004-0000-0500-00009A000000}"/>
-    <hyperlink ref="D72" r:id="rId68" xr:uid="{00000000-0004-0000-0500-00009B000000}"/>
-    <hyperlink ref="D73" r:id="rId69" xr:uid="{00000000-0004-0000-0500-00009C000000}"/>
-    <hyperlink ref="D74" r:id="rId70" xr:uid="{00000000-0004-0000-0500-00009D000000}"/>
-    <hyperlink ref="D75" r:id="rId71" xr:uid="{00000000-0004-0000-0500-00009E000000}"/>
-    <hyperlink ref="D76" r:id="rId72" xr:uid="{00000000-0004-0000-0500-00009F000000}"/>
-    <hyperlink ref="D77" r:id="rId73" xr:uid="{00000000-0004-0000-0500-0000A0000000}"/>
-    <hyperlink ref="D78" r:id="rId74" xr:uid="{00000000-0004-0000-0500-0000A1000000}"/>
-    <hyperlink ref="D79" r:id="rId75" xr:uid="{00000000-0004-0000-0500-0000A2000000}"/>
-    <hyperlink ref="D80" r:id="rId76" xr:uid="{00000000-0004-0000-0500-0000A3000000}"/>
-    <hyperlink ref="D81" r:id="rId77" xr:uid="{00000000-0004-0000-0500-0000A4000000}"/>
-    <hyperlink ref="D82" r:id="rId78" xr:uid="{00000000-0004-0000-0500-0000A5000000}"/>
-    <hyperlink ref="D83" r:id="rId79" xr:uid="{00000000-0004-0000-0500-0000A6000000}"/>
-    <hyperlink ref="D84" r:id="rId80" xr:uid="{00000000-0004-0000-0500-0000A7000000}"/>
-    <hyperlink ref="D85" r:id="rId81" xr:uid="{00000000-0004-0000-0500-0000A8000000}"/>
-    <hyperlink ref="D86" r:id="rId82" xr:uid="{00000000-0004-0000-0500-0000A9000000}"/>
-    <hyperlink ref="D87" r:id="rId83" xr:uid="{00000000-0004-0000-0500-0000AA000000}"/>
-    <hyperlink ref="D88" r:id="rId84" xr:uid="{00000000-0004-0000-0500-0000AB000000}"/>
-    <hyperlink ref="D89" r:id="rId85" xr:uid="{00000000-0004-0000-0500-0000AC000000}"/>
-    <hyperlink ref="D22" r:id="rId86" xr:uid="{00000000-0004-0000-0500-0000AD000000}"/>
-    <hyperlink ref="D7" r:id="rId87" xr:uid="{00000000-0004-0000-0500-0000AE000000}"/>
-    <hyperlink ref="A6" r:id="rId88" xr:uid="{D34B9DFE-CAF2-4002-8A75-3E88C785FE73}"/>
-    <hyperlink ref="A3" r:id="rId89" xr:uid="{D55DCEF1-58E9-49CD-A306-EC2B0696913C}"/>
-    <hyperlink ref="A40" r:id="rId90" xr:uid="{255BFEF2-EA0B-48DD-AE6A-A1E4F5F554E0}"/>
-    <hyperlink ref="A37" r:id="rId91" xr:uid="{CAA540D3-6BEE-4229-A977-8E8D8F8885A4}"/>
-    <hyperlink ref="A14" r:id="rId92" xr:uid="{8F56FDB6-B749-4472-A173-68692AB56915}"/>
-    <hyperlink ref="A28" r:id="rId93" xr:uid="{109B1F43-1243-417B-941D-E496A2A093A8}"/>
-    <hyperlink ref="A47" r:id="rId94" xr:uid="{3874B9EB-2CBF-4C6B-8F13-149322316408}"/>
-    <hyperlink ref="A53" r:id="rId95" xr:uid="{725311D9-B8BF-4922-90EC-D5D8E78083DD}"/>
-    <hyperlink ref="A55" r:id="rId96" xr:uid="{240F5350-5B92-451C-818B-02F6D13E3BAA}"/>
-    <hyperlink ref="E69" r:id="rId97" xr:uid="{57E52675-2220-49AA-876F-C78370CAB07B}"/>
-    <hyperlink ref="E56" r:id="rId98" xr:uid="{7BED298F-EEA1-4144-9433-7D514F1D86B8}"/>
-    <hyperlink ref="A57" r:id="rId99" xr:uid="{A040D5B5-CA92-40A5-9B22-62819B210ACC}"/>
-    <hyperlink ref="A71" r:id="rId100" xr:uid="{70239190-F5CF-403A-80B5-CAAB6A9D570A}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+    <hyperlink ref="D6" r:id="rId5"/>
+    <hyperlink ref="D8" r:id="rId6"/>
+    <hyperlink ref="D10" r:id="rId7"/>
+    <hyperlink ref="D11" r:id="rId8"/>
+    <hyperlink ref="D12" r:id="rId9"/>
+    <hyperlink ref="D13" r:id="rId10"/>
+    <hyperlink ref="D14" r:id="rId11"/>
+    <hyperlink ref="D15" r:id="rId12" display="http://www.linkedin.com/in/anushkjoshi"/>
+    <hyperlink ref="D16" r:id="rId13"/>
+    <hyperlink ref="D17" r:id="rId14"/>
+    <hyperlink ref="D18" r:id="rId15"/>
+    <hyperlink ref="D19" r:id="rId16" display="http://linkedin.com/in/arjama-mohanty-17616a243"/>
+    <hyperlink ref="D20" r:id="rId17"/>
+    <hyperlink ref="D21" r:id="rId18"/>
+    <hyperlink ref="D23" r:id="rId19"/>
+    <hyperlink ref="D24" r:id="rId20"/>
+    <hyperlink ref="D25" r:id="rId21"/>
+    <hyperlink ref="D26" r:id="rId22"/>
+    <hyperlink ref="D27" r:id="rId23"/>
+    <hyperlink ref="D28" r:id="rId24"/>
+    <hyperlink ref="D29" r:id="rId25"/>
+    <hyperlink ref="D30" r:id="rId26"/>
+    <hyperlink ref="D31" r:id="rId27"/>
+    <hyperlink ref="D32" r:id="rId28"/>
+    <hyperlink ref="D33" r:id="rId29" display="http://www.linkedin.com/in/priya-gadariya-a21312248"/>
+    <hyperlink ref="D34" r:id="rId30"/>
+    <hyperlink ref="D36" r:id="rId31"/>
+    <hyperlink ref="D37" r:id="rId32"/>
+    <hyperlink ref="D38" r:id="rId33"/>
+    <hyperlink ref="D39" r:id="rId34" display="http://linkedin.com/in/jinhal-maheshwari-71a217212/"/>
+    <hyperlink ref="D40" r:id="rId35"/>
+    <hyperlink ref="D41" r:id="rId36"/>
+    <hyperlink ref="D42" r:id="rId37" display="http://linkedin.in/in/kevalkanpariya"/>
+    <hyperlink ref="D43" r:id="rId38"/>
+    <hyperlink ref="D44" r:id="rId39"/>
+    <hyperlink ref="D45" r:id="rId40"/>
+    <hyperlink ref="D46" r:id="rId41"/>
+    <hyperlink ref="D47" r:id="rId42"/>
+    <hyperlink ref="D48" r:id="rId43"/>
+    <hyperlink ref="D49" r:id="rId44"/>
+    <hyperlink ref="D50" r:id="rId45"/>
+    <hyperlink ref="D51" r:id="rId46"/>
+    <hyperlink ref="D52" r:id="rId47"/>
+    <hyperlink ref="D53" r:id="rId48"/>
+    <hyperlink ref="D54" r:id="rId49" display="http://www.linkedin.com/in/nishank-sudhir-654924228"/>
+    <hyperlink ref="D55" r:id="rId50"/>
+    <hyperlink ref="D56" r:id="rId51"/>
+    <hyperlink ref="D57" r:id="rId52" display="https://in.linkedin.com/in/pragnesh-barik"/>
+    <hyperlink ref="D58" r:id="rId53"/>
+    <hyperlink ref="D59" r:id="rId54" display="https://pranitsatpute.com/"/>
+    <hyperlink ref="D60" r:id="rId55"/>
+    <hyperlink ref="D61" r:id="rId56"/>
+    <hyperlink ref="D62" r:id="rId57"/>
+    <hyperlink ref="D63" r:id="rId58"/>
+    <hyperlink ref="D64" r:id="rId59"/>
+    <hyperlink ref="D65" r:id="rId60"/>
+    <hyperlink ref="D66" r:id="rId61"/>
+    <hyperlink ref="D67" r:id="rId62"/>
+    <hyperlink ref="D68" r:id="rId63"/>
+    <hyperlink ref="D69" r:id="rId64"/>
+    <hyperlink ref="D70" r:id="rId65"/>
+    <hyperlink ref="D71" r:id="rId66"/>
+    <hyperlink ref="D72" r:id="rId67"/>
+    <hyperlink ref="D73" r:id="rId68"/>
+    <hyperlink ref="D74" r:id="rId69"/>
+    <hyperlink ref="D75" r:id="rId70"/>
+    <hyperlink ref="D76" r:id="rId71"/>
+    <hyperlink ref="D77" r:id="rId72"/>
+    <hyperlink ref="D78" r:id="rId73"/>
+    <hyperlink ref="D79" r:id="rId74"/>
+    <hyperlink ref="D80" r:id="rId75"/>
+    <hyperlink ref="D81" r:id="rId76"/>
+    <hyperlink ref="D82" r:id="rId77"/>
+    <hyperlink ref="D83" r:id="rId78"/>
+    <hyperlink ref="D84" r:id="rId79"/>
+    <hyperlink ref="D85" r:id="rId80"/>
+    <hyperlink ref="D86" r:id="rId81"/>
+    <hyperlink ref="D87" r:id="rId82"/>
+    <hyperlink ref="D88" r:id="rId83"/>
+    <hyperlink ref="D89" r:id="rId84"/>
+    <hyperlink ref="D90" r:id="rId85"/>
+    <hyperlink ref="D22" r:id="rId86"/>
+    <hyperlink ref="D7" r:id="rId87"/>
+    <hyperlink ref="A6" r:id="rId88"/>
+    <hyperlink ref="A3" r:id="rId89"/>
+    <hyperlink ref="A41" r:id="rId90"/>
+    <hyperlink ref="A38" r:id="rId91"/>
+    <hyperlink ref="A14" r:id="rId92"/>
+    <hyperlink ref="A28" r:id="rId93"/>
+    <hyperlink ref="A48" r:id="rId94"/>
+    <hyperlink ref="A54" r:id="rId95"/>
+    <hyperlink ref="A56" r:id="rId96"/>
+    <hyperlink ref="E70" r:id="rId97"/>
+    <hyperlink ref="E57" r:id="rId98"/>
+    <hyperlink ref="A58" r:id="rId99"/>
+    <hyperlink ref="A72" r:id="rId100"/>
+    <hyperlink ref="A35" r:id="rId101"/>
+    <hyperlink ref="D35" r:id="rId102"/>
+    <hyperlink ref="E35" r:id="rId103"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId101"/>
+  <pageSetup orientation="portrait" r:id="rId104"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Program Officers to Team page
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Github\Final NSS Website\src\components\Pages\Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\Desktop\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DAEFBF0-17D5-425F-9090-9C82549878C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508" activeTab="5"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
-    <sheet name="Founder" sheetId="2" r:id="rId2"/>
-    <sheet name="CoFounder" sheetId="3" r:id="rId3"/>
-    <sheet name="Team2019" sheetId="4" r:id="rId4"/>
-    <sheet name="Team2020" sheetId="5" r:id="rId5"/>
-    <sheet name="Team2021" sheetId="6" r:id="rId6"/>
+    <sheet name="ProgramCoordinators" sheetId="7" r:id="rId2"/>
+    <sheet name="Founder" sheetId="2" r:id="rId3"/>
+    <sheet name="CoFounder" sheetId="3" r:id="rId4"/>
+    <sheet name="Team2019" sheetId="4" r:id="rId5"/>
+    <sheet name="Team2020" sheetId="5" r:id="rId6"/>
+    <sheet name="Team2021" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="739">
   <si>
     <t>image</t>
   </si>
@@ -2202,13 +2204,52 @@
   </si>
   <si>
     <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2021%2FHarshit%20Pathak.jpg?alt=media&amp;token=5340d13d-1341-4d10-9105-e9b9263a8174</t>
+  </si>
+  <si>
+    <t>ritambhara.jangir@chem.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2Fprogram%20officers%2Frithambarimaam.jpg?alt=media&amp;token=55d35e5c-1f39-4dd9-8459-4be2edde5884</t>
+  </si>
+  <si>
+    <t>Dr Yogendra Kuwar</t>
+  </si>
+  <si>
+    <t>Dr. Ritambhara Jangir</t>
+  </si>
+  <si>
+    <t>yvk@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2Fprogram%20officers%2FYogendra%20Sir.jpg?alt=media&amp;token=288b61d2-181b-4e38-9dbf-52c710c95e8b</t>
+  </si>
+  <si>
+    <t>Dr. Aeidapu Mahesh</t>
+  </si>
+  <si>
+    <t>Dr. Shail Pandey</t>
+  </si>
+  <si>
+    <t>sp@phy.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>aeidapumahesh@eed.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>Program Officer</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2Fprogram%20officers%2FMahesh%20Adeipu.jpg?alt=media&amp;token=4dddbf5b-bee2-45cd-97a6-b839140c8b21</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2Fprogram%20officers%2FShail_pandey.jpeg?alt=media&amp;token=341a4d04-4a9d-4363-b483-e90bb7cede84</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2268,6 +2309,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2277,7 +2325,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -2307,12 +2355,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2359,7 +2418,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2369,10 +2427,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{C0E40833-B59F-493F-A45D-09F6C9D048B0}"/>
+    <cellStyle name="Normal 3" xfId="3" xr:uid="{43F2E9B4-3D35-4D50-8157-D15C00F531B8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2671,14 +2736,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection sqref="A1:V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2688,7 +2753,7 @@
     <col min="3" max="3" width="18.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="58.44140625" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2737,7 +2802,128 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A01B6ED-AB1B-43F1-AB4D-8CDBE46082FB}">
+  <dimension ref="A1:U5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.5546875" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="30.21875" customWidth="1"/>
+    <col min="4" max="4" width="39.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>724</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+    </row>
+    <row r="2" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>729</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>726</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>728</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>730</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>735</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>736</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>734</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>738</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:U1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{9AF73727-5991-4E8C-93A8-AED8CBBBD90F}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{3A43D525-80D3-48E0-8D91-B9E0CEC6459E}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{55045EE0-F6A6-4139-9C8E-A4B21DDD2B4D}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{F801B8D5-E80D-4581-A5CA-A42026514B9E}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{0E24DE5D-E8D6-47C0-A6A4-F44066BED909}"/>
+    <hyperlink ref="D4" r:id="rId6" xr:uid="{4EA994CF-1792-46C1-84CF-6835B2463B41}"/>
+    <hyperlink ref="D5" r:id="rId7" xr:uid="{20CC5B07-5D9D-4F03-A518-BF9DB79D640D}"/>
+    <hyperlink ref="C3" r:id="rId8" xr:uid="{59C1ADD7-4D4D-47BA-A25B-0ABAAABE554D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2754,23 +2940,23 @@
     <col min="3" max="3" width="14.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.5546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
@@ -2781,16 +2967,16 @@
       <c r="A2" s="4" t="s">
         <v>712</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>713</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>714</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="17" t="s">
         <v>715</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>716</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -2802,15 +2988,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2820,7 +3006,7 @@
     <col min="3" max="3" width="13" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="145" style="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32.6640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5546875" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2864,7 +3050,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="18" t="s">
         <v>695</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2944,12 +3130,15 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{E3205834-E1CD-4DB7-9C13-EE290B2D7383}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -3526,14 +3715,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F1040"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -12328,14 +12517,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:F1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E26" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
@@ -13030,7 +13219,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19" t="s">
+      <c r="A35" s="18" t="s">
         <v>171</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -21935,7 +22124,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A35" r:id="rId1"/>
+    <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
removed linkedin of Sir
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\Desktop\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0DAEFBF0-17D5-425F-9090-9C82549878C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D73F61-F38E-487D-9B2D-49F86EDF4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="920" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="738">
   <si>
     <t>image</t>
   </si>
@@ -2189,9 +2189,6 @@
   </si>
   <si>
     <t>Faculty Advisor</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/dr-bade-mukund-h-svnit-6b90ab261/</t>
   </si>
   <si>
     <t>bmh@med.svnit.ac.in</t>
@@ -2427,11 +2424,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2740,10 +2737,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2756,7 +2753,7 @@
     <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2767,16 +2764,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>724</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="13" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>718</v>
       </c>
@@ -2786,14 +2780,11 @@
       <c r="C2" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>721</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>722</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A01B6ED-AB1B-43F1-AB4D-8CDBE46082FB}">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
+    <sheetView zoomScale="84" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2827,81 +2818,81 @@
       <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>724</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
+      <c r="D1" s="20" t="s">
+        <v>723</v>
+      </c>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
     </row>
     <row r="2" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>725</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>726</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>727</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>729</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>730</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>731</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>734</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>736</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>735</v>
-      </c>
-      <c r="D4" s="21" t="s">
-        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>732</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>735</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>733</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>736</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>734</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>738</v>
+      <c r="D5" s="19" t="s">
+        <v>737</v>
       </c>
     </row>
   </sheetData>
@@ -2960,7 +2951,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3026,7 +3017,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3175,7 +3166,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -3753,7 +3744,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -12555,7 +12546,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -13235,7 +13226,7 @@
         <v>174</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Flipbook and updated team data
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\Desktop\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D73F61-F38E-487D-9B2D-49F86EDF4E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA242B5C-CC66-4BBB-A4BF-6EC16E62F7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>tapariyaaditi23@gmail.com</t>
   </si>
   <si>
-    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2021%2FAditi%20tapariya.jpg?alt=media&amp;token=8a4becc5-9979-4f19-b60e-05a61a7727f9</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/1x9apUlUtwJGT5Tph8hnxQhZoRGDLQpUj/view?usp=drive_link</t>
   </si>
   <si>
@@ -2240,6 +2237,9 @@
   </si>
   <si>
     <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2Fprogram%20officers%2FShail_pandey.jpeg?alt=media&amp;token=341a4d04-4a9d-4363-b483-e90bb7cede84</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2021%2FAditi%20Tapariya.jpg?alt=media&amp;token=b7a460ae-7e8a-4db5-badd-8e689c68f164</t>
   </si>
 </sst>
 </file>
@@ -2739,7 +2739,7 @@
   </sheetPr>
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -2767,24 +2767,24 @@
         <v>4</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>717</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>718</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="5" t="s">
         <v>721</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>722</v>
       </c>
     </row>
   </sheetData>
@@ -2819,7 +2819,7 @@
         <v>4</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
@@ -2841,58 +2841,58 @@
     </row>
     <row r="2" spans="1:21" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C2" s="18" t="s">
+        <v>724</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>725</v>
-      </c>
-      <c r="D2" s="19" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="C3" s="18" t="s">
+        <v>728</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>729</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>733</v>
+      </c>
+      <c r="D4" s="19" t="s">
         <v>735</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>734</v>
-      </c>
-      <c r="D4" s="19" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="C5" s="18" t="s">
         <v>732</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>733</v>
-      </c>
       <c r="D5" s="19" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
   </sheetData>
@@ -2951,27 +2951,27 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>712</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="16" t="s">
         <v>713</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>714</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>715</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="F2" s="5" t="s">
         <v>716</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>717</v>
       </c>
     </row>
   </sheetData>
@@ -3017,107 +3017,107 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>693</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
+        <v>694</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>695</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>662</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>697</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>700</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>701</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>704</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>705</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>707</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>690</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>708</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>691</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>709</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>710</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>711</v>
       </c>
     </row>
   </sheetData>
@@ -3166,227 +3166,227 @@
         <v>4</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>635</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>636</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>638</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>641</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>642</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>644</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>645</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>646</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>647</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>649</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>650</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>651</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>652</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>654</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>655</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>656</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>657</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>659</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>660</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>662</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>664</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>665</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>666</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>667</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>668</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>669</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>670</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>671</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>672</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>674</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>675</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>676</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>677</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>679</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>680</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>681</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="5" t="s">
         <v>682</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>684</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>685</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>686</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>687</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3744,747 +3744,747 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>451</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>452</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="5" t="s">
         <v>453</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>456</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>458</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>460</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>461</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>462</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="5" t="s">
         <v>463</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>466</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="5" t="s">
         <v>468</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>469</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>470</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>471</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>473</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>475</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>476</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>477</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>478</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>479</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>480</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>481</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>482</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>483</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>485</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>486</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>488</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>491</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>493</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>495</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>496</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>497</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="5" t="s">
         <v>498</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>501</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>503</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>506</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>508</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>510</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>511</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>512</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="5" t="s">
         <v>513</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>515</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>516</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>517</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>518</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>520</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>521</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="5" t="s">
         <v>523</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>525</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>527</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="5" t="s">
         <v>528</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>531</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="5" t="s">
         <v>533</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>535</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>536</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>538</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>540</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>541</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>542</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="5" t="s">
         <v>543</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>546</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>547</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="5" t="s">
         <v>548</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>549</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>550</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>551</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="5" t="s">
         <v>553</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>556</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>558</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>560</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>561</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="5" t="s">
         <v>563</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>565</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>566</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>566</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="5" t="s">
         <v>568</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>571</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="5" t="s">
         <v>573</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>575</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>576</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="5" t="s">
         <v>578</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>581</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="5" t="s">
         <v>583</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>585</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>586</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>587</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="5" t="s">
         <v>588</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>592</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="5" t="s">
         <v>593</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>595</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>596</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>597</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="5" t="s">
         <v>598</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>600</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>601</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>602</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="5" t="s">
         <v>603</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>604</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>605</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>606</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>607</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="5" t="s">
         <v>608</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>610</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>611</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>612</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="5" t="s">
         <v>613</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>615</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>616</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>617</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" s="5" t="s">
         <v>618</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>621</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>622</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="5" t="s">
         <v>623</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>625</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>626</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="5" t="s">
         <v>628</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>630</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>631</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>632</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="5" t="s">
         <v>633</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -12515,8 +12515,8 @@
   </sheetPr>
   <dimension ref="A1:F1063"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P38" sqref="P38"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12546,7 +12546,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -12645,1688 +12645,1688 @@
       <c r="E6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>30</v>
+      <c r="F6" s="19" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="5" t="s">
         <v>49</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="5" t="s">
         <v>54</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>62</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="5" t="s">
         <v>79</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="5" t="s">
         <v>84</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>101</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D21" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="5" t="s">
         <v>104</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>116</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>117</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="5" t="s">
         <v>119</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>121</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>122</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="5" t="s">
         <v>124</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="5" t="s">
         <v>134</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>137</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="5" t="s">
         <v>139</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>142</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D31" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="5" t="s">
         <v>154</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D33" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="F33" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>167</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D34" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="5" t="s">
         <v>169</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D35" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E35" s="4" t="s">
-        <v>174</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="F36" s="5" t="s">
         <v>178</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>181</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D37" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="F37" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D38" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="F38" s="5" t="s">
         <v>188</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="F39" s="5" t="s">
         <v>193</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D40" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="F40" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>201</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D41" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="F41" s="5" t="s">
         <v>203</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D42" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="F42" s="5" t="s">
         <v>208</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>210</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>211</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D43" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="F43" s="5" t="s">
         <v>213</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>216</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="F44" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>221</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D45" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="E45" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="F45" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>226</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D46" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="E46" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="F46" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F47" s="5" t="s">
         <v>233</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>235</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>236</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D48" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="F48" s="5" t="s">
         <v>238</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>241</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D49" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E49" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="F49" s="5" t="s">
         <v>243</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>246</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D50" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="F50" s="5" t="s">
         <v>248</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B51" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="E51" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="F51" s="5" t="s">
         <v>253</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="B52" s="2" t="s">
         <v>255</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D52" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="F52" s="5" t="s">
         <v>258</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D53" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="F53" s="5" t="s">
         <v>263</v>
-      </c>
-      <c r="F53" s="5" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="B54" s="2" t="s">
         <v>265</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>266</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D54" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="F54" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="F54" s="5" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B55" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>271</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D55" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="E55" s="2" t="s">
+      <c r="F55" s="5" t="s">
         <v>273</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D56" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E56" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="F56" s="5" t="s">
         <v>278</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="B57" s="2" t="s">
         <v>280</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>281</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D57" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="E57" s="4" t="s">
+      <c r="F57" s="5" t="s">
         <v>283</v>
-      </c>
-      <c r="F57" s="5" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="B58" s="2" t="s">
         <v>285</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>286</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D58" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E58" s="2" t="s">
         <v>287</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="F58" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="B59" s="2" t="s">
         <v>290</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>291</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D59" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E59" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="F59" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>295</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>296</v>
       </c>
       <c r="C60" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D60" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="F60" s="5" t="s">
         <v>298</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="B61" s="2" t="s">
         <v>300</v>
-      </c>
-      <c r="B61" s="2" t="s">
-        <v>301</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D61" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="E61" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="5" t="s">
         <v>303</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="B62" s="2" t="s">
         <v>305</v>
-      </c>
-      <c r="B62" s="2" t="s">
-        <v>306</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="E62" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>310</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>311</v>
       </c>
       <c r="C63" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D63" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="E63" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="5" t="s">
         <v>313</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>315</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>316</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D64" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E64" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="E64" s="2" t="s">
+      <c r="F64" s="5" t="s">
         <v>318</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B65" s="2" t="s">
         <v>320</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>321</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="E65" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="E65" s="2" t="s">
+      <c r="F65" s="5" t="s">
         <v>323</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D66" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="F66" s="5" t="s">
         <v>328</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="B67" s="2" t="s">
         <v>330</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>331</v>
       </c>
       <c r="C67" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D67" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>332</v>
       </c>
-      <c r="E67" s="2" t="s">
+      <c r="F67" s="5" t="s">
         <v>333</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="B68" s="2" t="s">
         <v>335</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>336</v>
       </c>
       <c r="C68" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D68" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="E68" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="F68" s="5" t="s">
         <v>338</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>340</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>341</v>
       </c>
       <c r="C69" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D69" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="E69" s="2" t="s">
         <v>342</v>
       </c>
-      <c r="E69" s="2" t="s">
+      <c r="F69" s="5" t="s">
         <v>343</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="B70" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="B70" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="E70" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="E70" s="4" t="s">
+      <c r="F70" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B71" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="B71" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D71" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E71" s="2" t="s">
         <v>352</v>
       </c>
-      <c r="E71" s="2" t="s">
+      <c r="F71" s="5" t="s">
         <v>353</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>355</v>
-      </c>
-      <c r="B72" s="2" t="s">
-        <v>356</v>
       </c>
       <c r="C72" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D72" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E72" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="F72" s="5" t="s">
         <v>358</v>
-      </c>
-      <c r="F72" s="5" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="B73" s="2" t="s">
         <v>360</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>361</v>
       </c>
       <c r="C73" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D73" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="E73" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="E73" s="2" t="s">
+      <c r="F73" s="5" t="s">
         <v>363</v>
-      </c>
-      <c r="F73" s="5" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="B74" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="B74" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="C74" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D74" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E74" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E74" s="2" t="s">
+      <c r="F74" s="5" t="s">
         <v>368</v>
-      </c>
-      <c r="F74" s="5" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="B75" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="C75" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D75" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="E75" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="E75" s="2" t="s">
+      <c r="F75" s="5" t="s">
         <v>373</v>
-      </c>
-      <c r="F75" s="5" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="B76" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="B76" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D76" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="E76" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="E76" s="2" t="s">
+      <c r="F76" s="5" t="s">
         <v>378</v>
-      </c>
-      <c r="F76" s="5" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="B77" s="2" t="s">
         <v>380</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>381</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D77" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E77" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="F77" s="5" t="s">
         <v>383</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="C78" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D78" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E78" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="F78" s="5" t="s">
         <v>388</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>390</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>391</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D79" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="E79" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="E79" s="2" t="s">
+      <c r="F79" s="5" t="s">
         <v>393</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>395</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>396</v>
       </c>
       <c r="C80" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D80" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="E80" s="2" t="s">
         <v>397</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="5" t="s">
         <v>398</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="B81" s="2" t="s">
         <v>400</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>401</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D81" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="E81" s="2" t="s">
         <v>402</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="5" t="s">
         <v>403</v>
-      </c>
-      <c r="F81" s="5" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="B82" s="2" t="s">
         <v>405</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>406</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D82" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E82" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="5" t="s">
         <v>408</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="B83" s="2" t="s">
         <v>410</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>411</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D83" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="E83" s="2" t="s">
         <v>412</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="5" t="s">
         <v>413</v>
-      </c>
-      <c r="F83" s="5" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B84" s="2" t="s">
         <v>415</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>416</v>
       </c>
       <c r="C84" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D84" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="E84" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" s="5" t="s">
         <v>418</v>
-      </c>
-      <c r="F84" s="5" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>420</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>421</v>
       </c>
       <c r="C85" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D85" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="E85" s="2" t="s">
         <v>422</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="5" t="s">
         <v>423</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="B86" s="2" t="s">
         <v>425</v>
-      </c>
-      <c r="B86" s="2" t="s">
-        <v>426</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D86" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="E86" s="2" t="s">
         <v>427</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="5" t="s">
         <v>428</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="B87" s="2" t="s">
         <v>430</v>
-      </c>
-      <c r="B87" s="2" t="s">
-        <v>431</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D87" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="E87" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="5" t="s">
         <v>433</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>435</v>
-      </c>
-      <c r="B88" s="2" t="s">
-        <v>436</v>
       </c>
       <c r="C88" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D88" s="4" t="s">
+        <v>436</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="F88" s="5" t="s">
         <v>438</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B89" s="2" t="s">
         <v>440</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>441</v>
       </c>
       <c r="C89" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D89" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="E89" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="F89" s="5" t="s">
         <v>443</v>
-      </c>
-      <c r="F89" s="5" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>446</v>
       </c>
       <c r="C90" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D90" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E90" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="5" t="s">
         <v>448</v>
-      </c>
-      <c r="F90" s="5" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -22116,6 +22116,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A35" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{179F4BE2-CF0A-4086-97DC-721B5CDE7031}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Script to Automatically Upload Team Data.
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\Desktop\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA242B5C-CC66-4BBB-A4BF-6EC16E62F7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96043A31-4B05-4006-A1B7-0742BE4C94B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -20,13 +20,14 @@
     <sheet name="Team2019" sheetId="4" r:id="rId5"/>
     <sheet name="Team2020" sheetId="5" r:id="rId6"/>
     <sheet name="Team2021" sheetId="6" r:id="rId7"/>
+    <sheet name="Team2022" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="948">
   <si>
     <t>image</t>
   </si>
@@ -2240,13 +2241,643 @@
   </si>
   <si>
     <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2021%2FAditi%20Tapariya.jpg?alt=media&amp;token=b7a460ae-7e8a-4db5-badd-8e689c68f164</t>
+  </si>
+  <si>
+    <t>Badme</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1a4tMoCIwnG7-BD34A3zGikwhzqjcg-T_</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ansh-dwivedi-146494251?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>anshdwivedi611@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10P1XyLXQOIIXPvWr3D0nm9ZbI8Yt0uV-</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vaibhav-vispute-2134a724a?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>vaibhavvspt273@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1WKy_vsNJGNbOz65bnU_8NpI7MhGy0Cea</t>
+  </si>
+  <si>
+    <t>Dilipkumar kalsariya</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dk-ahir-303474283?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>dilipkalsariya22@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17Bse8QvLACVO6_53aZ6sfgIal_TD0t7j</t>
+  </si>
+  <si>
+    <t>u22ee075@eed.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>Amisha soni</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/amisha-soni-6716722b1?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10fNGUa977Si5MFh3Vgc2nADl503I_10X</t>
+  </si>
+  <si>
+    <t>harsh-rai-277370273</t>
+  </si>
+  <si>
+    <t>hrai7706@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1jpIb4Rvyle4R77ckubA1br5oKpBbdDro</t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>shivamkaimur2k2@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1kMxH2Gif6A8xOwpLkc-ziCInfv8xRaRM</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/raja-singh-313147177?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>rsingh10111nits@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1kI1GYD2cGRDC2HLM4nTSGIrrNQlxgOEa</t>
+  </si>
+  <si>
+    <t>Abhinav Anand</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abhinav-anand-5a2611292?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>anandabhinav2003@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1rkZAna-6N6C1TfYhh0IaTwqdDxpir1TY</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vinit-soni-813639332</t>
+  </si>
+  <si>
+    <t>vinitsoni073@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1GYSuZtV2QcZ1hJeqysbqXhPcirDWt1IJ</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/stuti-singh-20255a253?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>Sstuti276@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1mPjklLiCAb_nSNppHS_hxWvxcqutOFxS</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1i_JVvp2NsLYB6igp25rUlDGmNDUhhj9A</t>
+  </si>
+  <si>
+    <t>Bodepu Harika</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/bodepu-harika-901ba624a/</t>
+  </si>
+  <si>
+    <t>harika.bodepu2005@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1XLqo0g6XzftmuAG86RBUmnZ_ETPjjmqm</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ashishrajput0904/</t>
+  </si>
+  <si>
+    <t>rajputashishsingh018@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16r4uP4Tx42qTi58Q6qTXJ-rr9qkoCnBx</t>
+  </si>
+  <si>
+    <t>Ayukta Labh</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ayukta-labh-776469283</t>
+  </si>
+  <si>
+    <t>ayuktalabh@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10wcxnUz9S6U6A_KZDVVvSl4vr1EybIC8</t>
+  </si>
+  <si>
+    <t>Vikram Poonia</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/vikrampoonia107</t>
+  </si>
+  <si>
+    <t>vikrampoonia107@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1mRg7DoSzlTzqBqw4kZUYR_5d__N-_9Le</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/himani-gupta-05210425a?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>himuu0904@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=103qlSyZL8CqsPN40zw0zRwBhDwV3U2rD</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/neelima-kadimisetti-830609258?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>neelimakadimisetti@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1CUYRdOHPZJVv8Cc2_zMkBXtDj54W7o3h</t>
+  </si>
+  <si>
+    <t>u22ce052@ced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>Ajay kr Rajak</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/ajay-kr-rajak-755b99263/</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1U1wdy3tqJ9FzgORI4VjkSCpCyq9cKbE_</t>
+  </si>
+  <si>
+    <t>Vidhan Gauswami</t>
+  </si>
+  <si>
+    <t>vidhan.gauswami@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1SXFAU2JcK9v10v2qZ4owmWHy2eLzbhfu</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/burhanuddin-dadawala-57b830288?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=</t>
+  </si>
+  <si>
+    <t>Burhanzakir07@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=124WVO7sKJvppay12rKqfASUAux7bMw2P</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/rongali-balaji-36916a289/</t>
+  </si>
+  <si>
+    <t>balajirongali0504@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=15li_PZ83lX3YfQPHj6ckh0YWjOgznqlK</t>
+  </si>
+  <si>
+    <t>u22ec125@eced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/meetchudasama</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=13eNA_M-2HoGT3dTofNEGdHpAsDiFyMax</t>
+  </si>
+  <si>
+    <t>Veeravalli Haritha</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/haritha-veeravalli-b22818258?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>harithaveeravalli20@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1e4thr-36wEJ49y1ubxP7n-Ti6yC2XQhn</t>
+  </si>
+  <si>
+    <t>Maahir Malde</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/maahir-malde/</t>
+  </si>
+  <si>
+    <t>maldemaahir@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17APq9m0MfM4jw9SpWKgVKG2vqBdpsFOw</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/lakshmidurga-saladi-a9b28528a?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>lakshmidurgasaladi4@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ZDfQpzh2cwJwJdB8sgOHU63ljakX3vRx</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/aashish-gupta-2b4aa9326?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>aashishg8160@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1cKtaOwSi0VAcC5fYW140NBKWVdWrpQov</t>
+  </si>
+  <si>
+    <t>Pawan Shukla</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/pawan-shukla-36pds29</t>
+  </si>
+  <si>
+    <t>pkscmshukla1313@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1qliKdwnejf-hAV6p9ZCHAd_AFcW70P-G</t>
+  </si>
+  <si>
+    <t>Na</t>
+  </si>
+  <si>
+    <t>rj645231@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1-G6KbfLHVkphoRG3C6DPXJV6JwZ33Dq1</t>
+  </si>
+  <si>
+    <t>Eswar Pesala</t>
+  </si>
+  <si>
+    <t>pesalaeswar7@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1m_FxWgVulWqIVelv20pjYIBmf7vg45qa</t>
+  </si>
+  <si>
+    <t>u22ce098@ced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/naina-bansal-5b5859253</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=14aXrUvgq4BELgTvsT4HpLfFxGLAGYDBo</t>
+  </si>
+  <si>
+    <t>Misbah Shaikh</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/misbahsrshaikh/</t>
+  </si>
+  <si>
+    <t>misbahsrshaikh@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1B_TAy7OzGHusB8Cl7dDqXigJlzgroH8y</t>
+  </si>
+  <si>
+    <t>u22me147@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>Nancy Agrawal</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=13yDtGkcxFgg-A7zID9_Qc5QDLDPCe2AF</t>
+  </si>
+  <si>
+    <t>Honey Bohra</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/honey-bohra-38322a261</t>
+  </si>
+  <si>
+    <t>honeybohra26@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=181usj7XFakGdyBQOVxYGmmVAxLOKl28R</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/ divyesh-pankhaniya</t>
+  </si>
+  <si>
+    <t>divyeshjpankhaniya022@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1pLsqhT36MhOO3vqnn3UjyXSY6tVX_bRQ</t>
+  </si>
+  <si>
+    <t>Devanshi Thaker</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/devanshi-thaker-4a18a7257?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>devanshi2034@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1QY0uo8frPUGkFqGrfufmnMXxcY1-eHRn</t>
+  </si>
+  <si>
+    <t>Adarsh Tiwari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/adarshtiwari25?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>adarshtiwari2505@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1fbEQhO9OP-rp6SDj87hbghPbV5aw0wAb</t>
+  </si>
+  <si>
+    <t>u22ec079@eced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/chaitanya-singh-b771b2254?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10iMMzmNA3ZVcoclT6QGeJtXiBM-VrrPW</t>
+  </si>
+  <si>
+    <t>Eshaan Goel</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/eshaan-goel-0361a2256?trk=contact-info</t>
+  </si>
+  <si>
+    <t>eshaangoel2503@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1CfD4Uas-HaJpgyxXeaNx-uwnh3ildQtX</t>
+  </si>
+  <si>
+    <t>u22me021@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>TIWARI OM SURESHKUMAR</t>
+  </si>
+  <si>
+    <t>https://in.linkedin.com/in/omtiwari0000</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IGNOcwDbasAoNMkhPYNoCAckwJzLn3ef</t>
+  </si>
+  <si>
+    <t>Puneet Tiwari</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/puneet-tiwari-8bb0a22a6</t>
+  </si>
+  <si>
+    <t>U22ec015@eced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=121OB-0s-K4-KcA1pCH2TrWL0i22tf_CA</t>
+  </si>
+  <si>
+    <t>Sonam</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sonam-mehra-b19b42293?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>elintsonam70996@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1F8-xP2_Oi3nTp--J29Z_A0Yo_Sz_WCAc</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/in/bolle-ranjith-901771285</t>
+  </si>
+  <si>
+    <t>ranjithbolle13@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=13kgu5IDerEkit-PbiO_Oc6TGjFT8dv79</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/adarsh-kumar-srivastava-b48641248?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>adarshsrivastava450@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1y4HACVUO9DihD3M9eBOagq35_PXvtitJ</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=174yE4Lg8Ipc1HsapQgn-V5jVINryY3f1</t>
+  </si>
+  <si>
+    <t>u22me217@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>Aanchal Kumari</t>
+  </si>
+  <si>
+    <t>http://linkedin.com/in/aanchalkumari93</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1mnrcqecNYr31ALecbV0elsRlqc6DKSLJ</t>
+  </si>
+  <si>
+    <t>u22ce099@ced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1eOrmjPX2SXsL2wID6vyfVDkselF-SplA</t>
+  </si>
+  <si>
+    <t>Ashish mehra</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/a04b30251</t>
+  </si>
+  <si>
+    <t>ashishmehra8690@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1QwqnV63CI9vT-cy7M8mr1Zl38yiYhOHt</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IE_Z2cQOt3aSx8MKt375xzQbmLH_BCzW</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1p729DCvU_OLtwhM0Q9GvGpedUhhH4wQp</t>
+  </si>
+  <si>
+    <t>Shrishti Arya</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shrishtiarya</t>
+  </si>
+  <si>
+    <t>shrishtiarya2004@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1Az-U1f62uhdpf0YfX8OsMSt0fB4Y0z-a</t>
+  </si>
+  <si>
+    <t>Nivas</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/nivas1426</t>
+  </si>
+  <si>
+    <t>nnivas235@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1h0ZiAnMveKlht89G3zJa8LtlVoDBIK5o</t>
+  </si>
+  <si>
+    <t>Dilipkumar Kalsariya</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dilipkumar-kalsariya-303474283?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=10JvUvDeZ4sC1C7nQ8m3dC0pDOBP4oS_7</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1TY5x8kV1YqMWGHANDjQsYJTvzIFrKW-G</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1rpUtJliD8h8UPth4swjLoZuAS82Xv_iz</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=15g0caxnOpj_yK5axI2DBKUZnmF2NfnIr</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sneha-vishnoi-80a1222b1?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>snehvi22@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1dwMTHC0ABIsQBiON3RE8EIkse8vAsbBq</t>
+  </si>
+  <si>
+    <t>Samarth Chaplot</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/samarth-chaplot-130b88256/</t>
+  </si>
+  <si>
+    <t>samarthchaplot7@gmail.com</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1pZ39G3Jmxzqmu5qbKKYMUQyVEx2R5JCY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ansh Dwivedi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaibhav Suresh Vispute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harsh Rai </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shivam Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raja Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VINIT SONI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuti Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">STUTI SINGH </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ashish Rajput </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Himani gupta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kadimisetti Neelima </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vidhan Gauswami </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burhanuddin Dadawala </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balaji Rongali </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meet Kumar Chudasama </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lakshmi durga saladi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aashish Gupta </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rishabh jain </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naina bansal </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divyesh Pankhaniya </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chaitanya Singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">B Ranjith </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adarsh Kumar Srivastava </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subham kumar </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stuti singh </t>
+  </si>
+  <si>
+    <t xml:space="preserve">VIDHAN GAUSWAMI </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneha Vishnoi </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Na </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.linkedin.com/in/pesala-eswar-485031262</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2313,16 +2944,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor rgb="FFF8F9FA"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2361,6 +3017,96 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF442F65"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF8F9FA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2368,7 +3114,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2429,6 +3175,33 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3135,7 +3908,7 @@
   </sheetPr>
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -3713,7 +4486,7 @@
   </sheetPr>
   <dimension ref="A1:F1040"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="105" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -12515,8 +13288,8 @@
   </sheetPr>
   <dimension ref="A1:F1063"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -22120,4 +22893,1297 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B711C-931B-4692-9EDF-C6704E3B4B67}">
+  <dimension ref="A1:F90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79.6640625" customWidth="1"/>
+    <col min="2" max="2" width="50.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" customWidth="1"/>
+    <col min="4" max="4" width="142.33203125" customWidth="1"/>
+    <col min="5" max="5" width="41.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>739</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>938</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>738</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="29" t="s">
+        <v>742</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>919</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>740</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
+        <v>745</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>920</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>743</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="s">
+        <v>749</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>746</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>747</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>753</v>
+      </c>
+      <c r="B6" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="29" t="s">
+        <v>756</v>
+      </c>
+      <c r="B7" s="23" t="s">
+        <v>921</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>754</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>759</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>922</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>757</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="29" t="s">
+        <v>762</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>923</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>760</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>766</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29" t="s">
+        <v>769</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>924</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>767</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>772</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>925</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="26" t="s">
+        <v>770</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="29" t="s">
+        <v>773</v>
+      </c>
+      <c r="B13" s="23" t="s">
+        <v>926</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>770</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>777</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>774</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>775</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="29" t="s">
+        <v>780</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>927</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>778</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>784</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>781</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="26" t="s">
+        <v>782</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>788</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>785</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>786</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>791</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>928</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>789</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="29" t="s">
+        <v>794</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>929</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>792</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>798</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>796</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>797</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="29" t="s">
+        <v>801</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>930</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>799</v>
+      </c>
+      <c r="E21" s="23" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>804</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>931</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>802</v>
+      </c>
+      <c r="E22" s="22" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="29" t="s">
+        <v>807</v>
+      </c>
+      <c r="B23" s="23" t="s">
+        <v>932</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>805</v>
+      </c>
+      <c r="E23" s="23" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>810</v>
+      </c>
+      <c r="B24" s="22" t="s">
+        <v>933</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>809</v>
+      </c>
+      <c r="E24" s="22" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="29" t="s">
+        <v>814</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>811</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>812</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>818</v>
+      </c>
+      <c r="B26" s="22" t="s">
+        <v>815</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>816</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="29" t="s">
+        <v>821</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>934</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>819</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>824</v>
+      </c>
+      <c r="B28" s="22" t="s">
+        <v>935</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="26" t="s">
+        <v>822</v>
+      </c>
+      <c r="E28" s="22" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="29" t="s">
+        <v>828</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>825</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>826</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>831</v>
+      </c>
+      <c r="B30" s="22" t="s">
+        <v>936</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="22" t="s">
+        <v>946</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="29" t="s">
+        <v>834</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>832</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>947</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>837</v>
+      </c>
+      <c r="B32" s="22" t="s">
+        <v>937</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="26" t="s">
+        <v>836</v>
+      </c>
+      <c r="E32" s="22" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="29" t="s">
+        <v>841</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>838</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>839</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="28" t="s">
+        <v>844</v>
+      </c>
+      <c r="B34" s="22" t="s">
+        <v>843</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="29" t="s">
+        <v>848</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>845</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>846</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>851</v>
+      </c>
+      <c r="B36" s="22" t="s">
+        <v>938</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="22" t="s">
+        <v>849</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="29" t="s">
+        <v>855</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>852</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>853</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="28" t="s">
+        <v>859</v>
+      </c>
+      <c r="B38" s="22" t="s">
+        <v>856</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="26" t="s">
+        <v>857</v>
+      </c>
+      <c r="E38" s="22" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="29" t="s">
+        <v>862</v>
+      </c>
+      <c r="B39" s="23" t="s">
+        <v>939</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>861</v>
+      </c>
+      <c r="E39" s="23" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="28" t="s">
+        <v>866</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>864</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="29" t="s">
+        <v>870</v>
+      </c>
+      <c r="B41" s="23" t="s">
+        <v>868</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>869</v>
+      </c>
+      <c r="E41" s="23" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="28" t="s">
+        <v>874</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>871</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>872</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="29" t="s">
+        <v>878</v>
+      </c>
+      <c r="B43" s="23" t="s">
+        <v>875</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>876</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="28" t="s">
+        <v>881</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>940</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>879</v>
+      </c>
+      <c r="E44" s="22" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="29" t="s">
+        <v>884</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>941</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>882</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="28" t="s">
+        <v>885</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>924</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>767</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="29" t="s">
+        <v>889</v>
+      </c>
+      <c r="B47" s="23" t="s">
+        <v>887</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>888</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="28" t="s">
+        <v>891</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>942</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="29" t="s">
+        <v>895</v>
+      </c>
+      <c r="B49" s="23" t="s">
+        <v>892</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>893</v>
+      </c>
+      <c r="E49" s="23" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="28" t="s">
+        <v>896</v>
+      </c>
+      <c r="B50" s="22" t="s">
+        <v>751</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>752</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="29" t="s">
+        <v>897</v>
+      </c>
+      <c r="B51" s="23" t="s">
+        <v>928</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="25" t="s">
+        <v>789</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="28" t="s">
+        <v>901</v>
+      </c>
+      <c r="B52" s="22" t="s">
+        <v>898</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>899</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="29" t="s">
+        <v>905</v>
+      </c>
+      <c r="B53" s="23" t="s">
+        <v>902</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>903</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="28" t="s">
+        <v>908</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>906</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>907</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="29" t="s">
+        <v>909</v>
+      </c>
+      <c r="B55" s="23" t="s">
+        <v>943</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>770</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="28" t="s">
+        <v>910</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>763</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" s="26" t="s">
+        <v>764</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="29" t="s">
+        <v>911</v>
+      </c>
+      <c r="B57" s="23" t="s">
+        <v>944</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" s="23" t="s">
+        <v>829</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="28" t="s">
+        <v>914</v>
+      </c>
+      <c r="B58" s="22" t="s">
+        <v>945</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>912</v>
+      </c>
+      <c r="E58" s="22" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="30" t="s">
+        <v>918</v>
+      </c>
+      <c r="B59" s="24" t="s">
+        <v>915</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="27" t="s">
+        <v>916</v>
+      </c>
+      <c r="E59" s="24" t="s">
+        <v>917</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C60" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C61" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C62" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C63" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C64" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C65" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C66" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C67" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C68" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C69" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C70" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C71" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C72" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C73" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C74" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C76" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C77" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C78" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C79" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C80" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C81" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C82" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C83" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C84" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C85" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C86" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C87" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C88" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C89" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C90" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D59" r:id="rId1" xr:uid="{C88148CF-5DF9-4253-B76C-4E1CBD8BC84D}"/>
+    <hyperlink ref="D58" r:id="rId2" xr:uid="{8E16E620-9CC3-4E63-9AC2-FD0A420760BD}"/>
+    <hyperlink ref="D56" r:id="rId3" xr:uid="{D8B40303-4817-4250-9E13-60D18E5D93E3}"/>
+    <hyperlink ref="D55" r:id="rId4" xr:uid="{E91FD67D-0D32-469E-A247-6C4FAF32E067}"/>
+    <hyperlink ref="D54" r:id="rId5" xr:uid="{7BB0E27A-0711-4B5F-93B3-7D03BEC26951}"/>
+    <hyperlink ref="D53" r:id="rId6" xr:uid="{832606AC-B272-40E7-BF42-106ED7E88224}"/>
+    <hyperlink ref="D52" r:id="rId7" xr:uid="{3FA31C2C-C945-42B8-9FF4-BD59AA7110C0}"/>
+    <hyperlink ref="D51" r:id="rId8" xr:uid="{75A3865D-4A79-401A-BAB5-50C8B38FD8DD}"/>
+    <hyperlink ref="D50" r:id="rId9" xr:uid="{6FBCBD0D-4B21-4B38-87A3-82A37CE2C8A6}"/>
+    <hyperlink ref="D49" r:id="rId10" xr:uid="{8131EEDE-EEAE-42B7-AEE4-2EA2F9EAF1A5}"/>
+    <hyperlink ref="D47" r:id="rId11" xr:uid="{4E6674DF-2000-41F4-8472-3F662E16F814}"/>
+    <hyperlink ref="D46" r:id="rId12" xr:uid="{2D30A9D1-ED9F-4CA0-A53B-77E3BBEC3DB1}"/>
+    <hyperlink ref="D45" r:id="rId13" xr:uid="{8217C29A-744F-4FEE-9428-12D4582D5415}"/>
+    <hyperlink ref="D44" r:id="rId14" xr:uid="{F89E0BDE-119E-4FB0-A10E-CBA20EAA14AB}"/>
+    <hyperlink ref="D43" r:id="rId15" xr:uid="{A5279A3F-20FE-49BF-86AE-E3A37C8D8686}"/>
+    <hyperlink ref="D42" r:id="rId16" xr:uid="{5CF8102E-222F-490D-927F-4F5D1DBE2B09}"/>
+    <hyperlink ref="D41" r:id="rId17" xr:uid="{EF248E29-FB43-4091-BDB4-37112C5985BE}"/>
+    <hyperlink ref="D40" r:id="rId18" xr:uid="{EF9A1364-4133-4DC4-A10A-80D978B935AB}"/>
+    <hyperlink ref="D39" r:id="rId19" xr:uid="{CC933F2F-5DED-409A-9966-791069A17C63}"/>
+    <hyperlink ref="D38" r:id="rId20" xr:uid="{79B9C70D-532C-443F-80C3-9D164D4AD827}"/>
+    <hyperlink ref="D37" r:id="rId21" xr:uid="{7026003E-68F9-4056-A3D9-510E646DB2C7}"/>
+    <hyperlink ref="D35" r:id="rId22" xr:uid="{B32B0029-894F-4FA6-80AC-975F68F6E772}"/>
+    <hyperlink ref="D33" r:id="rId23" xr:uid="{52D53C68-AF36-4696-AD13-8D60403CC314}"/>
+    <hyperlink ref="D32" r:id="rId24" xr:uid="{E5EE4567-832F-4896-B69F-A3E6BED15C7E}"/>
+    <hyperlink ref="D31" r:id="rId25" xr:uid="{735D4054-D99B-43FA-BB19-9F74CA4789D4}"/>
+    <hyperlink ref="D29" r:id="rId26" xr:uid="{A376F93A-64F9-4823-AF9E-E370A1F9AAEF}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{0FC92F16-2F84-492A-AB86-9966BD3231BA}"/>
+    <hyperlink ref="D27" r:id="rId28" xr:uid="{7816835E-1F73-41CC-8723-483484C10A18}"/>
+    <hyperlink ref="D26" r:id="rId29" xr:uid="{206531C1-798E-4854-BF46-4D8D5931B511}"/>
+    <hyperlink ref="D25" r:id="rId30" xr:uid="{ABCC6629-C8AD-4FD5-BB89-C9CFEA17E4AD}"/>
+    <hyperlink ref="D24" r:id="rId31" xr:uid="{484DD7C9-89D3-4052-BB5D-9ADB6389CC99}"/>
+    <hyperlink ref="D23" r:id="rId32" xr:uid="{AA10BF32-3043-4BB9-81FE-1D405364442C}"/>
+    <hyperlink ref="D22" r:id="rId33" xr:uid="{9CA7CD20-61FC-4961-BEA1-40E1CA448B47}"/>
+    <hyperlink ref="D20" r:id="rId34" xr:uid="{55AFE04B-22ED-4A46-A876-645CF9F862ED}"/>
+    <hyperlink ref="D19" r:id="rId35" xr:uid="{E1BA6F41-F6E5-4B03-93C2-90569ED52F49}"/>
+    <hyperlink ref="D18" r:id="rId36" xr:uid="{AC59A219-424E-4C53-8D43-6DAAB862FA99}"/>
+    <hyperlink ref="D17" r:id="rId37" xr:uid="{1305D2F3-E4CB-4784-8782-8CBE56332A40}"/>
+    <hyperlink ref="D16" r:id="rId38" xr:uid="{876519C2-3E8B-4272-AF83-08A0D76DA628}"/>
+    <hyperlink ref="D15" r:id="rId39" xr:uid="{685DDD16-694A-4EF3-A7FF-F68E6CAD8BE4}"/>
+    <hyperlink ref="D14" r:id="rId40" xr:uid="{634BF867-9D93-45AF-8C0A-7CA45376C73D}"/>
+    <hyperlink ref="D13" r:id="rId41" xr:uid="{084DA96A-7929-46E2-BC7B-63F419F7C68D}"/>
+    <hyperlink ref="D12" r:id="rId42" xr:uid="{5912C85B-34AA-42DA-84F4-7C0085B3E496}"/>
+    <hyperlink ref="D11" r:id="rId43" xr:uid="{D23CA796-F210-471A-BEF8-1FF4B56E38DA}"/>
+    <hyperlink ref="D10" r:id="rId44" xr:uid="{BBDD90AF-88A7-44B4-A045-52BB6B51F83F}"/>
+    <hyperlink ref="D9" r:id="rId45" xr:uid="{7616D031-03AC-4A61-833A-E940D432D045}"/>
+    <hyperlink ref="D6" r:id="rId46" xr:uid="{D820B794-41E8-4872-B328-EB6B355F968E}"/>
+    <hyperlink ref="D5" r:id="rId47" xr:uid="{98FE490F-65B9-4816-BC45-42099885484D}"/>
+    <hyperlink ref="D4" r:id="rId48" xr:uid="{6F8AC833-7AD7-421B-98BD-F74E60CEE2B0}"/>
+    <hyperlink ref="D3" r:id="rId49" xr:uid="{93599FED-EC9E-4FEE-A16A-1623CEB8CC2C}"/>
+    <hyperlink ref="A59" r:id="rId50" xr:uid="{D7BCC3F4-9E98-4352-A19C-712FA78AD17A}"/>
+    <hyperlink ref="A58" r:id="rId51" xr:uid="{12EFF059-D100-473C-8B0B-6C836D6F0F0E}"/>
+    <hyperlink ref="A57" r:id="rId52" xr:uid="{83C531B8-3F29-4DE0-8D89-ED0A5ACDAF07}"/>
+    <hyperlink ref="A56" r:id="rId53" xr:uid="{183B6974-EF45-48E6-B1E2-02DD7DA50A8B}"/>
+    <hyperlink ref="A55" r:id="rId54" xr:uid="{2BB77A6D-578C-4576-9E7B-5FA730E7D7ED}"/>
+    <hyperlink ref="A54" r:id="rId55" xr:uid="{200BC5ED-9F43-4788-A057-2B8AC41BFB82}"/>
+    <hyperlink ref="A53" r:id="rId56" xr:uid="{15284D7E-66E8-41A5-8140-F94175FF5EB3}"/>
+    <hyperlink ref="A52" r:id="rId57" xr:uid="{EFD97A66-76B3-4F61-8873-68E761E6542C}"/>
+    <hyperlink ref="A51" r:id="rId58" xr:uid="{596E175E-19F2-4264-92FD-5A5444BBDD2D}"/>
+    <hyperlink ref="A50" r:id="rId59" xr:uid="{D6D834B8-34F1-43F8-B8F7-EB3F88F62D03}"/>
+    <hyperlink ref="A49" r:id="rId60" xr:uid="{FC728830-2146-4871-907F-A003556C7CCA}"/>
+    <hyperlink ref="A48" r:id="rId61" xr:uid="{EC1AFD13-0F72-4D33-8E4F-4885D424A87C}"/>
+    <hyperlink ref="A47" r:id="rId62" xr:uid="{F4BDE8B7-494C-49A2-80E3-FAAC607F2943}"/>
+    <hyperlink ref="A46" r:id="rId63" xr:uid="{1A3FDEB5-17F1-4127-8DD4-46AE795635BE}"/>
+    <hyperlink ref="A45" r:id="rId64" xr:uid="{8319DB39-0463-4291-BF1B-70C3A2F062A1}"/>
+    <hyperlink ref="A44" r:id="rId65" xr:uid="{B900F8B6-4304-48E5-B5B4-F073FC936AC8}"/>
+    <hyperlink ref="A43" r:id="rId66" xr:uid="{94AB4193-D457-4F4E-ACA6-B3C2F5018E95}"/>
+    <hyperlink ref="A42" r:id="rId67" xr:uid="{C8DC4A00-F4A9-4790-B67B-B55AA1F944A6}"/>
+    <hyperlink ref="A41" r:id="rId68" xr:uid="{AF0645BB-AAC6-42FE-B22E-7CAB07872D4E}"/>
+    <hyperlink ref="A40" r:id="rId69" xr:uid="{ED7021DF-F409-4450-B262-8519E3684CF2}"/>
+    <hyperlink ref="A39" r:id="rId70" xr:uid="{0700FCEA-0E9B-4E34-8EAF-F88C145D097E}"/>
+    <hyperlink ref="A38" r:id="rId71" xr:uid="{4FA06A04-AD92-4F99-85DA-67C63E67162E}"/>
+    <hyperlink ref="A37" r:id="rId72" xr:uid="{A6910EF4-50CC-4489-B5EF-F35F86ED2E34}"/>
+    <hyperlink ref="A36" r:id="rId73" xr:uid="{6FB0C2D4-3284-465D-A8DC-7E529B7D8B5D}"/>
+    <hyperlink ref="A35" r:id="rId74" xr:uid="{E3D046A9-484F-4787-A32A-BDBE04D2C3B1}"/>
+    <hyperlink ref="A34" r:id="rId75" xr:uid="{E1C3B582-1BC7-47BC-99F4-6186688F19AA}"/>
+    <hyperlink ref="A33" r:id="rId76" xr:uid="{9B1F3C9E-D31E-4E2D-8FD2-BB41C7D3A1C7}"/>
+    <hyperlink ref="A32" r:id="rId77" xr:uid="{28DFF2F9-4BDF-449E-8F0C-712A1A84C851}"/>
+    <hyperlink ref="A31" r:id="rId78" xr:uid="{2C63D54B-C00A-4A32-8C35-29686A08CB33}"/>
+    <hyperlink ref="A30" r:id="rId79" xr:uid="{8477D1E0-4351-4D25-99BE-F8BC90B849BC}"/>
+    <hyperlink ref="A29" r:id="rId80" xr:uid="{03BA8D29-DD43-4F3F-AA57-A1A418C1979A}"/>
+    <hyperlink ref="A28" r:id="rId81" xr:uid="{118D02C2-EAC2-491D-8DC5-2DD8B396AD3A}"/>
+    <hyperlink ref="A27" r:id="rId82" xr:uid="{FAC169D1-B1AF-4A3A-B5FA-1E225000F3DC}"/>
+    <hyperlink ref="A26" r:id="rId83" xr:uid="{C825A856-920B-407D-A727-B2ADC04659A1}"/>
+    <hyperlink ref="A25" r:id="rId84" xr:uid="{1785FCE4-B50E-4AF6-83B4-254D49C5E735}"/>
+    <hyperlink ref="A24" r:id="rId85" xr:uid="{903D5FCB-7E16-4D6C-A6E8-F35403F542E5}"/>
+    <hyperlink ref="A23" r:id="rId86" xr:uid="{3D113737-8792-4CD0-B164-09858C165D30}"/>
+    <hyperlink ref="A22" r:id="rId87" xr:uid="{85BF75BE-1717-4BB5-94D0-4ABE948DE249}"/>
+    <hyperlink ref="A21" r:id="rId88" xr:uid="{E6B34616-1684-4173-BF2C-D14034DA4AA5}"/>
+    <hyperlink ref="A20" r:id="rId89" xr:uid="{9FBBB347-2468-4CF5-BBD4-BBE359ED8C6B}"/>
+    <hyperlink ref="A19" r:id="rId90" xr:uid="{ADDC7CE5-8811-4F9D-9DDF-DFC253D6874F}"/>
+    <hyperlink ref="A18" r:id="rId91" xr:uid="{E24F9448-B953-4718-9B43-458499B8CE7C}"/>
+    <hyperlink ref="A17" r:id="rId92" xr:uid="{4C6247D2-1D84-4B47-B378-B87B2A2C2993}"/>
+    <hyperlink ref="A16" r:id="rId93" xr:uid="{633AF3BA-8A29-4EF1-9CB5-970A53DA7689}"/>
+    <hyperlink ref="A15" r:id="rId94" xr:uid="{8689DBBA-9120-4067-882F-8AB44609F825}"/>
+    <hyperlink ref="A14" r:id="rId95" xr:uid="{A32B1C44-D580-4A9C-BA5C-2E2A701F515A}"/>
+    <hyperlink ref="A13" r:id="rId96" xr:uid="{9521E09C-42B5-4AE2-A532-7B9720832CC1}"/>
+    <hyperlink ref="A12" r:id="rId97" xr:uid="{E5CD8BF2-74D9-4117-80B3-A29C1B984E48}"/>
+    <hyperlink ref="A11" r:id="rId98" xr:uid="{2862C1A3-5995-453D-89CB-E9B00CDAE5E3}"/>
+    <hyperlink ref="A10" r:id="rId99" xr:uid="{5ADCF538-0B36-4963-BCC5-057D83C260C9}"/>
+    <hyperlink ref="A9" r:id="rId100" xr:uid="{92167A81-22F3-44B6-8351-46A4DDBE954C}"/>
+    <hyperlink ref="A8" r:id="rId101" xr:uid="{B308E0AB-A3EE-4795-BD76-974B32A46402}"/>
+    <hyperlink ref="A7" r:id="rId102" xr:uid="{E7F5FDFB-8A4D-4375-B9BC-CC2475F03189}"/>
+    <hyperlink ref="A6" r:id="rId103" xr:uid="{10B9B3AC-33AF-440A-AFB4-72CE640FD25B}"/>
+    <hyperlink ref="A5" r:id="rId104" xr:uid="{2FD40AE4-FDDE-4685-AB16-4E239BC66426}"/>
+    <hyperlink ref="A4" r:id="rId105" xr:uid="{0C6F8E01-DB72-454C-BA9C-3C4956675A52}"/>
+    <hyperlink ref="A3" r:id="rId106" xr:uid="{D3365FDF-D8C2-4E7C-B47D-B866014F1AF0}"/>
+    <hyperlink ref="A2" r:id="rId107" xr:uid="{B8DE23EB-9A10-45E9-A865-51E8D23193B5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId108"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
team page 2022 updated
</commit_message>
<xml_diff>
--- a/src/components/Pages/Team/Team_data.xlsx
+++ b/src/components/Pages/Team/Team_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samarth\Desktop\NSS-WEBSITE\src\components\Pages\Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somu\Desktop\Nss website\NSS-WEBSITE\src\components\Pages\Team\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7753EAD-1C2B-4C8B-B371-E7230388C06C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F2B08B-B14B-49F2-B0A7-8A5A86FF217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sir" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="976">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1248" uniqueCount="1005">
   <si>
     <t>image</t>
   </si>
@@ -2955,13 +2955,100 @@
   </si>
   <si>
     <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FVISPUTE%20VAIBHAV%20SURESH%20SVNIT.jpg?alt=media&amp;token=6e3bb491-bbd4-411b-a805-847444a99d8d</t>
+  </si>
+  <si>
+    <t>Burhanuddin Dadawala</t>
+  </si>
+  <si>
+    <t>Dharti Chauhan</t>
+  </si>
+  <si>
+    <t>Gaurav Nambiar</t>
+  </si>
+  <si>
+    <t>Shiv Pratap Singh</t>
+  </si>
+  <si>
+    <t>TIWARI OM SURESHKUMAR</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/burhanuddin-dadawala-57b830288?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=</t>
+  </si>
+  <si>
+    <t>https://in.linkedin.com/in/omtiwari0000</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/shiv-pratap-singh-44a868290?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/dharti-chauhan-8027a4282</t>
+  </si>
+  <si>
+    <t>u22me174@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>u22ce087@ced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>u22ce093@ced.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>u22me199@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>u22me021@med.svnit.ac.in</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=124WVO7sKJvppay12rKqfASUAux7bMw2P</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17VnJntQSmnL2klfz5tdt-Fji1ybub0Nj</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1pZd8kPEXFvYfJ23xylUaI-xkUHkCxbOA</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1m92HgpTkiPSbMUWiKeE4f7g6eWnzZ-E1</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1IGNOcwDbasAoNMkhPYNoCAckwJzLn3ef</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FBURHANUDDIN%20DADAWALA.png?alt=media&amp;token=256b2725-9299-42de-ae19-eefee469922e</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FCHAUHAN%20DHARTI%20JAGDISH%20SVNIT.jpeg?alt=media&amp;token=d54ad5da-f66a-4eae-9f9c-564398cfe742</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FNAMBIAR%20GAURAV%20GOPINATH%20SVNIT.jpg?alt=media&amp;token=724b7c2f-2afd-42d3-8438-2023a85a598a</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FSHIV%20PRATAP%20SINGH%20SVNIT.jpg?alt=media&amp;token=d3a0b65f-60b5-4b0d-9c35-d9bd87b477f1</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FTIWARI%20OM%20SURESHKUMAR%20SVNIT.jpg?alt=media&amp;token=fb95809b-c8e1-4c78-acc7-d4cde3347a3b</t>
+  </si>
+  <si>
+    <t>C:\Users\somu\Desktop\Nss website\NSS-WEBSITE\src\components\Pages\Team\Team_data.xlsx</t>
+  </si>
+  <si>
+    <t>Kunal Kumar</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/kunal-kumar-570016265?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>kumarkunal102003@gmail.com</t>
+  </si>
+  <si>
+    <t>https://firebasestorage.googleapis.com/v0/b/nss-svnit.appspot.com/o/team%20page%2F2022%2FKunalKumar.jpg?alt=media&amp;token=02020ea8-9b27-4145-b6d3-edd871aa79ca</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3041,8 +3128,24 @@
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF434343"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3061,8 +3164,20 @@
         <bgColor rgb="FFF8F9FA"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F9FA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -3193,13 +3308,62 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFCCCCCC"/>
+        <color rgb="FFF8F9FA"/>
       </left>
       <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
         <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFF8F9FA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFF8F9FA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF442F65"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFF8F9FA"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -3209,7 +3373,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3274,25 +3438,16 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="8" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3323,20 +3478,96 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3726,26 +3957,26 @@
       <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="59"/>
+      <c r="Q1" s="59"/>
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="59"/>
     </row>
     <row r="2" spans="1:21" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -3834,7 +4065,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="68.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="91.109375" style="15" customWidth="1"/>
     <col min="2" max="2" width="16.5546875" style="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="38.33203125" style="15" bestFit="1" customWidth="1"/>
@@ -13423,7 +13654,7 @@
   </sheetPr>
   <dimension ref="A1:F1063"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D11" zoomScale="55" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1:C90"/>
     </sheetView>
   </sheetViews>
@@ -23032,23 +23263,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="114" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.6640625" customWidth="1"/>
+    <col min="1" max="1" width="158.21875" customWidth="1"/>
     <col min="2" max="2" width="50.44140625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
-    <col min="4" max="4" width="142.33203125" customWidth="1"/>
+    <col min="4" max="4" width="161" customWidth="1"/>
     <col min="5" max="5" width="41.44140625" customWidth="1"/>
     <col min="6" max="6" width="227.5546875" customWidth="1"/>
+    <col min="7" max="7" width="56.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -23068,108 +23300,109 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="27" t="s">
         <v>738</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="29" t="s">
         <v>739</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" s="34" t="s">
+      <c r="D2" s="31" t="s">
         <v>740</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="29" t="s">
         <v>741</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="37" t="s">
         <v>973</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+    <row r="3" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
         <v>742</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="30" t="s">
         <v>743</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="32" t="s">
         <v>744</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="30" t="s">
         <v>745</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="37" t="s">
         <v>974</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="31" t="s">
+    <row r="4" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="28" t="s">
         <v>746</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="30" t="s">
         <v>747</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="32" t="s">
         <v>748</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="30" t="s">
         <v>749</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="37" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="27" t="s">
         <v>750</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>751</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>752</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="29" t="s">
         <v>753</v>
       </c>
-      <c r="F5" s="44" t="s">
-        <v>928</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="31" t="s">
+      <c r="F5" s="37" t="s">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
         <v>754</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="30" t="s">
         <v>755</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="32" t="s">
         <v>756</v>
       </c>
-      <c r="E6" s="33" t="s">
+      <c r="E6" s="30" t="s">
         <v>757</v>
       </c>
-      <c r="F6" s="44" t="s">
-        <v>929</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="26" t="s">
+      <c r="F6" s="37" t="s">
+        <v>928</v>
+      </c>
+      <c r="G6" s="37"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="24" t="s">
         <v>758</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -23178,38 +23411,38 @@
       <c r="C7" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>760</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>761</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="37" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="31" t="s">
+    <row r="8" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
         <v>762</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>763</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="32" t="s">
         <v>764</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="E8" s="30" t="s">
         <v>765</v>
       </c>
-      <c r="F8" s="44" t="s">
+      <c r="F8" s="37" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="26" t="s">
         <v>766</v>
       </c>
       <c r="B9" s="21" t="s">
@@ -23218,38 +23451,38 @@
       <c r="C9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="22" t="s">
         <v>768</v>
       </c>
       <c r="E9" s="21" t="s">
         <v>769</v>
       </c>
-      <c r="F9" s="44" t="s">
+      <c r="F9" s="37" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="30" t="s">
+    <row r="10" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="27" t="s">
         <v>770</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>771</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="D10" s="31" t="s">
         <v>772</v>
       </c>
-      <c r="E10" s="32" t="s">
+      <c r="E10" s="29" t="s">
         <v>773</v>
       </c>
       <c r="F10" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="27" t="s">
+    <row r="11" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
         <v>774</v>
       </c>
       <c r="B11" s="21" t="s">
@@ -23258,18 +23491,18 @@
       <c r="C11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>776</v>
       </c>
       <c r="E11" s="21" t="s">
         <v>777</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="F11" s="37" t="s">
         <v>958</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
         <v>778</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -23278,757 +23511,895 @@
       <c r="C12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="23" t="s">
         <v>780</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>781</v>
       </c>
-      <c r="F12" s="44" t="s">
+      <c r="F12" s="37" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="31" t="s">
+    <row r="13" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
         <v>782</v>
       </c>
-      <c r="B13" s="33" t="s">
+      <c r="B13" s="30" t="s">
         <v>783</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="32" t="s">
         <v>784</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" s="30" t="s">
         <v>785</v>
       </c>
       <c r="F13" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+    <row r="14" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="27" t="s">
         <v>786</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="29" t="s">
         <v>787</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="31" t="s">
         <v>788</v>
       </c>
-      <c r="E14" s="32" t="s">
+      <c r="E14" s="29" t="s">
         <v>789</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="37" t="s">
         <v>960</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31" t="s">
+    <row r="15" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
         <v>790</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="30" t="s">
         <v>791</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="32" t="s">
         <v>792</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="30" t="s">
         <v>793</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="37" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="27" t="s">
-        <v>794</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>795</v>
+    <row r="16" spans="1:7" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>990</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>976</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>796</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>797</v>
-      </c>
-      <c r="F16" s="44" t="s">
-        <v>937</v>
+      <c r="D16" s="51" t="s">
+        <v>981</v>
+      </c>
+      <c r="E16" s="54" t="s">
+        <v>985</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>995</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
-        <v>798</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>799</v>
+      <c r="A17" s="27" t="s">
+        <v>794</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>795</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="34" t="s">
-        <v>800</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>801</v>
-      </c>
-      <c r="F17" s="44" t="s">
-        <v>968</v>
+      <c r="D17" s="31" t="s">
+        <v>796</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>797</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>937</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="27" t="s">
-        <v>802</v>
+      <c r="A18" s="25" t="s">
+        <v>798</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>803</v>
+        <v>799</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="37" t="s">
-        <v>804</v>
+      <c r="D18" s="22" t="s">
+        <v>800</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>805</v>
-      </c>
-      <c r="F18" s="44" t="s">
-        <v>938</v>
+        <v>801</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>968</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="26" t="s">
-        <v>806</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>807</v>
+      <c r="A19" s="35" t="s">
+        <v>991</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>977</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D19" s="36" t="s">
-        <v>808</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>809</v>
+        <v>984</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>986</v>
       </c>
       <c r="F19" t="s">
-        <v>939</v>
+        <v>996</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="31" t="s">
-        <v>810</v>
-      </c>
-      <c r="B20" s="33" t="s">
-        <v>811</v>
+      <c r="A20" s="25" t="s">
+        <v>802</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>803</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="35" t="s">
-        <v>812</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>813</v>
-      </c>
-      <c r="F20" s="44" t="s">
-        <v>940</v>
+      <c r="D20" s="34" t="s">
+        <v>804</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>805</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>938</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30" t="s">
-        <v>814</v>
-      </c>
-      <c r="B21" s="32" t="s">
-        <v>815</v>
+      <c r="A21" s="24" t="s">
+        <v>806</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>807</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="34" t="s">
-        <v>816</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>817</v>
-      </c>
-      <c r="F21" s="44" t="s">
-        <v>955</v>
+      <c r="D21" s="33" t="s">
+        <v>808</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>809</v>
+      </c>
+      <c r="F21" s="57" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="27" t="s">
-        <v>818</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>819</v>
+      <c r="A22" s="28" t="s">
+        <v>810</v>
+      </c>
+      <c r="B22" s="30" t="s">
+        <v>811</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="21" t="s">
-        <v>820</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>821</v>
-      </c>
-      <c r="F22" s="44" t="s">
-        <v>944</v>
+      <c r="D22" s="32" t="s">
+        <v>812</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>813</v>
+      </c>
+      <c r="F22" s="37" t="s">
+        <v>940</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="26" t="s">
-        <v>822</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>823</v>
+      <c r="A23" s="27" t="s">
+        <v>814</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>815</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="24" t="s">
-        <v>824</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>825</v>
-      </c>
-      <c r="F23" s="44" t="s">
-        <v>942</v>
+      <c r="D23" s="31" t="s">
+        <v>816</v>
+      </c>
+      <c r="E23" s="29" t="s">
+        <v>817</v>
+      </c>
+      <c r="F23" s="37" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="30" t="s">
-        <v>826</v>
-      </c>
-      <c r="B24" s="32" t="s">
-        <v>827</v>
+      <c r="A24" s="35" t="s">
+        <v>992</v>
+      </c>
+      <c r="B24" s="50" t="s">
+        <v>978</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D24" s="34" t="s">
-        <v>828</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>829</v>
-      </c>
-      <c r="F24" s="44" t="s">
-        <v>945</v>
+      <c r="D24" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>987</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>997</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="27" t="s">
-        <v>830</v>
+      <c r="A25" s="25" t="s">
+        <v>818</v>
       </c>
       <c r="B25" s="21" t="s">
-        <v>831</v>
+        <v>819</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="23" t="s">
-        <v>832</v>
+      <c r="D25" s="21" t="s">
+        <v>820</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>833</v>
-      </c>
-      <c r="F25" s="44" t="s">
-        <v>946</v>
+        <v>821</v>
+      </c>
+      <c r="F25" s="37" t="s">
+        <v>944</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="38" t="s">
-        <v>834</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>835</v>
+      <c r="A26" s="24" t="s">
+        <v>822</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>823</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D26" s="43" t="s">
-        <v>836</v>
-      </c>
-      <c r="E26" s="40" t="s">
-        <v>837</v>
-      </c>
-      <c r="F26" s="44" t="s">
-        <v>972</v>
+      <c r="D26" s="23" t="s">
+        <v>824</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>825</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
-        <v>838</v>
+      <c r="A27" s="25" t="s">
+        <v>826</v>
       </c>
       <c r="B27" s="21" t="s">
-        <v>839</v>
+        <v>827</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>840</v>
+      <c r="D27" s="22" t="s">
+        <v>828</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>841</v>
-      </c>
-      <c r="F27" s="44" t="s">
-        <v>947</v>
+        <v>829</v>
+      </c>
+      <c r="F27" s="37" t="s">
+        <v>945</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="26" t="s">
-        <v>842</v>
-      </c>
-      <c r="B28" s="20" t="s">
-        <v>843</v>
+      <c r="A28" s="27" t="s">
+        <v>830</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>831</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D28" s="24" t="s">
-        <v>844</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>845</v>
-      </c>
-      <c r="F28" s="44" t="s">
-        <v>949</v>
+      <c r="D28" s="31" t="s">
+        <v>832</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>833</v>
+      </c>
+      <c r="F28" s="37" t="s">
+        <v>946</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="31" t="s">
-        <v>846</v>
-      </c>
-      <c r="B29" s="33" t="s">
-        <v>847</v>
+      <c r="A29" s="39" t="s">
+        <v>834</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>835</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="35" t="s">
-        <v>848</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>849</v>
-      </c>
-      <c r="F29" s="44" t="s">
-        <v>950</v>
+      <c r="D29" s="51" t="s">
+        <v>836</v>
+      </c>
+      <c r="E29" s="46" t="s">
+        <v>837</v>
+      </c>
+      <c r="F29" s="37" t="s">
+        <v>972</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="30" t="s">
-        <v>850</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>851</v>
+      <c r="A30" s="60" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B30" s="63" t="s">
+        <v>1001</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D30" s="34" t="s">
-        <v>852</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>853</v>
-      </c>
-      <c r="F30" s="44" t="s">
-        <v>948</v>
+      <c r="D30" s="37" t="s">
+        <v>1002</v>
+      </c>
+      <c r="E30" s="67" t="s">
+        <v>1003</v>
+      </c>
+      <c r="F30" s="37" t="s">
+        <v>1004</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="31" t="s">
-        <v>854</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>855</v>
+      <c r="A31" s="25" t="s">
+        <v>838</v>
+      </c>
+      <c r="B31" s="21" t="s">
+        <v>839</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D31" s="35" t="s">
-        <v>856</v>
-      </c>
-      <c r="E31" s="33" t="s">
-        <v>857</v>
-      </c>
-      <c r="F31" s="44" t="s">
-        <v>951</v>
+      <c r="D31" s="22" t="s">
+        <v>840</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>841</v>
+      </c>
+      <c r="F31" s="37" t="s">
+        <v>947</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="26" t="s">
-        <v>858</v>
+      <c r="A32" s="24" t="s">
+        <v>842</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>859</v>
+        <v>843</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>64</v>
+      <c r="D32" s="23" t="s">
+        <v>844</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>860</v>
-      </c>
-      <c r="F32" s="44" t="s">
-        <v>953</v>
+        <v>845</v>
+      </c>
+      <c r="F32" s="37" t="s">
+        <v>949</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="27" t="s">
-        <v>861</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>862</v>
+      <c r="A33" s="28" t="s">
+        <v>846</v>
+      </c>
+      <c r="B33" s="30" t="s">
+        <v>847</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>863</v>
-      </c>
-      <c r="E33" s="21" t="s">
-        <v>864</v>
-      </c>
-      <c r="F33" s="44" t="s">
-        <v>952</v>
+      <c r="D33" s="32" t="s">
+        <v>848</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>849</v>
+      </c>
+      <c r="F33" s="37" t="s">
+        <v>950</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="30" t="s">
-        <v>865</v>
-      </c>
-      <c r="B34" s="32" t="s">
-        <v>866</v>
+      <c r="A34" s="27" t="s">
+        <v>850</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>851</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D34" s="34" t="s">
-        <v>867</v>
-      </c>
-      <c r="E34" s="32" t="s">
-        <v>868</v>
-      </c>
-      <c r="F34" s="44" t="s">
-        <v>954</v>
+      <c r="D34" s="31" t="s">
+        <v>852</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>853</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>948</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="31" t="s">
-        <v>869</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>870</v>
+      <c r="A35" s="28" t="s">
+        <v>854</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>855</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="35" t="s">
-        <v>871</v>
-      </c>
-      <c r="E35" s="33" t="s">
-        <v>872</v>
-      </c>
-      <c r="F35" s="44" t="s">
-        <v>956</v>
+      <c r="D35" s="32" t="s">
+        <v>856</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>857</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>951</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="30" t="s">
-        <v>873</v>
-      </c>
-      <c r="B36" s="32" t="s">
-        <v>874</v>
+      <c r="A36" s="24" t="s">
+        <v>858</v>
+      </c>
+      <c r="B36" s="20" t="s">
+        <v>859</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="34" t="s">
-        <v>875</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>876</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>957</v>
+      <c r="D36" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>860</v>
+      </c>
+      <c r="F36" s="37" t="s">
+        <v>953</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="31" t="s">
-        <v>877</v>
-      </c>
-      <c r="B37" s="33" t="s">
-        <v>878</v>
+      <c r="A37" s="25" t="s">
+        <v>861</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>862</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D37" s="33" t="s">
-        <v>879</v>
-      </c>
-      <c r="E37" s="33" t="s">
-        <v>880</v>
-      </c>
-      <c r="F37" t="s">
-        <v>959</v>
+      <c r="D37" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>864</v>
+      </c>
+      <c r="F37" s="43" t="s">
+        <v>952</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="30" t="s">
-        <v>881</v>
-      </c>
-      <c r="B38" s="32" t="s">
-        <v>882</v>
+      <c r="A38" s="27" t="s">
+        <v>865</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>866</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D38" s="34" t="s">
-        <v>883</v>
-      </c>
-      <c r="E38" s="32" t="s">
-        <v>884</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>961</v>
+      <c r="D38" s="31" t="s">
+        <v>867</v>
+      </c>
+      <c r="E38" s="29" t="s">
+        <v>868</v>
+      </c>
+      <c r="F38" s="62" t="s">
+        <v>954</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="31" t="s">
-        <v>885</v>
-      </c>
-      <c r="B39" s="33" t="s">
-        <v>886</v>
+      <c r="A39" s="28" t="s">
+        <v>869</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>870</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>887</v>
-      </c>
-      <c r="E39" s="33" t="s">
-        <v>888</v>
-      </c>
-      <c r="F39" s="44" t="s">
-        <v>966</v>
+      <c r="D39" s="32" t="s">
+        <v>871</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>872</v>
+      </c>
+      <c r="F39" s="37" t="s">
+        <v>956</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="26" t="s">
-        <v>889</v>
-      </c>
-      <c r="B40" s="20" t="s">
-        <v>890</v>
+      <c r="A40" s="27" t="s">
+        <v>873</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>874</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D40" s="24" t="s">
-        <v>891</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>892</v>
-      </c>
-      <c r="F40" t="s">
-        <v>962</v>
+      <c r="D40" s="31" t="s">
+        <v>875</v>
+      </c>
+      <c r="E40" s="29" t="s">
+        <v>876</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="31" t="s">
-        <v>893</v>
-      </c>
-      <c r="B41" s="33" t="s">
-        <v>894</v>
+      <c r="A41" s="28" t="s">
+        <v>877</v>
+      </c>
+      <c r="B41" s="30" t="s">
+        <v>878</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="35" t="s">
-        <v>895</v>
-      </c>
-      <c r="E41" s="33" t="s">
-        <v>896</v>
-      </c>
-      <c r="F41" s="44" t="s">
-        <v>967</v>
+      <c r="D41" s="30" t="s">
+        <v>879</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>880</v>
+      </c>
+      <c r="F41" s="73" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="30" t="s">
-        <v>897</v>
-      </c>
-      <c r="B42" s="32" t="s">
-        <v>898</v>
+      <c r="A42" s="27" t="s">
+        <v>881</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>882</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D42" s="34" t="s">
-        <v>899</v>
-      </c>
-      <c r="E42" s="32" t="s">
-        <v>900</v>
-      </c>
-      <c r="F42" s="44" t="s">
-        <v>963</v>
+      <c r="D42" s="31" t="s">
+        <v>883</v>
+      </c>
+      <c r="E42" s="29" t="s">
+        <v>884</v>
+      </c>
+      <c r="F42" s="37" t="s">
+        <v>961</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="31" t="s">
-        <v>901</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>902</v>
+      <c r="A43" s="39" t="s">
+        <v>993</v>
+      </c>
+      <c r="B43" s="66" t="s">
+        <v>979</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="35" t="s">
-        <v>903</v>
-      </c>
-      <c r="E43" s="33" t="s">
-        <v>904</v>
-      </c>
-      <c r="F43" s="44" t="s">
-        <v>964</v>
+      <c r="D43" s="51" t="s">
+        <v>983</v>
+      </c>
+      <c r="E43" s="54" t="s">
+        <v>988</v>
+      </c>
+      <c r="F43" s="57" t="s">
+        <v>998</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="26" t="s">
-        <v>905</v>
+      <c r="A44" s="24" t="s">
+        <v>885</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>906</v>
+        <v>886</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>58</v>
       </c>
       <c r="D44" s="20" t="s">
-        <v>64</v>
+        <v>887</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>907</v>
-      </c>
-      <c r="F44" s="44" t="s">
-        <v>965</v>
+        <v>888</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>966</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="26" t="s">
-        <v>908</v>
+      <c r="A45" s="24" t="s">
+        <v>889</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>909</v>
+        <v>890</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D45" s="24" t="s">
-        <v>910</v>
+      <c r="D45" s="23" t="s">
+        <v>891</v>
       </c>
       <c r="E45" s="20" t="s">
-        <v>911</v>
-      </c>
-      <c r="F45" s="44" t="s">
-        <v>975</v>
+        <v>892</v>
+      </c>
+      <c r="F45" s="57" t="s">
+        <v>962</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="27" t="s">
-        <v>912</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>913</v>
+      <c r="A46" s="28" t="s">
+        <v>893</v>
+      </c>
+      <c r="B46" s="30" t="s">
+        <v>894</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>914</v>
-      </c>
-      <c r="E46" s="21" t="s">
-        <v>915</v>
-      </c>
-      <c r="F46" s="44" t="s">
-        <v>969</v>
+      <c r="D46" s="32" t="s">
+        <v>895</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>896</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>967</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="30" t="s">
-        <v>916</v>
-      </c>
-      <c r="B47" s="32" t="s">
-        <v>917</v>
+      <c r="A47" s="27" t="s">
+        <v>897</v>
+      </c>
+      <c r="B47" s="29" t="s">
+        <v>898</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D47" s="32" t="s">
-        <v>918</v>
-      </c>
-      <c r="E47" s="32" t="s">
-        <v>919</v>
-      </c>
-      <c r="F47" s="44" t="s">
-        <v>941</v>
+      <c r="D47" s="31" t="s">
+        <v>899</v>
+      </c>
+      <c r="E47" s="29" t="s">
+        <v>900</v>
+      </c>
+      <c r="F47" s="37" t="s">
+        <v>963</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28" t="s">
-        <v>920</v>
-      </c>
-      <c r="B48" s="22" t="s">
-        <v>921</v>
+      <c r="A48" s="42" t="s">
+        <v>901</v>
+      </c>
+      <c r="B48" s="49" t="s">
+        <v>902</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="25" t="s">
+      <c r="D48" s="70" t="s">
+        <v>903</v>
+      </c>
+      <c r="E48" s="49" t="s">
+        <v>904</v>
+      </c>
+      <c r="F48" s="43" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="61" t="s">
+        <v>905</v>
+      </c>
+      <c r="B49" s="64" t="s">
+        <v>906</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E49" s="64" t="s">
+        <v>907</v>
+      </c>
+      <c r="F49" s="43" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="62" t="s">
+        <v>994</v>
+      </c>
+      <c r="B50" s="65" t="s">
+        <v>980</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D50" s="62" t="s">
+        <v>982</v>
+      </c>
+      <c r="E50" s="72" t="s">
+        <v>989</v>
+      </c>
+      <c r="F50" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="40" t="s">
+        <v>908</v>
+      </c>
+      <c r="B51" s="45" t="s">
+        <v>909</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D51" s="40" t="s">
+        <v>910</v>
+      </c>
+      <c r="E51" s="71" t="s">
+        <v>911</v>
+      </c>
+      <c r="F51" s="43" t="s">
+        <v>975</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="41" t="s">
+        <v>912</v>
+      </c>
+      <c r="B52" s="48" t="s">
+        <v>913</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D52" s="69" t="s">
+        <v>914</v>
+      </c>
+      <c r="E52" s="53" t="s">
+        <v>915</v>
+      </c>
+      <c r="F52" s="43" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="41" t="s">
+        <v>916</v>
+      </c>
+      <c r="B53" s="48" t="s">
+        <v>917</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D53" s="68" t="s">
+        <v>918</v>
+      </c>
+      <c r="E53" s="56" t="s">
+        <v>919</v>
+      </c>
+      <c r="F53" s="43" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="41" t="s">
+        <v>920</v>
+      </c>
+      <c r="B54" s="48" t="s">
+        <v>921</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D54" s="41" t="s">
         <v>922</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E54" s="53" t="s">
         <v>923</v>
       </c>
-      <c r="F48" t="s">
+      <c r="F54" t="s">
         <v>970</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="39" t="s">
+    <row r="55" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="61" t="s">
         <v>924</v>
       </c>
-      <c r="B49" s="41" t="s">
+      <c r="B55" s="64" t="s">
         <v>925</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C55" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D55" s="61" t="s">
         <v>926</v>
       </c>
-      <c r="E49" s="41" t="s">
+      <c r="E55" s="64" t="s">
         <v>927</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F55" t="s">
         <v>971</v>
       </c>
     </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="37"/>
+    </row>
+    <row r="58" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="37"/>
+    </row>
+    <row r="59" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="38"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="37"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="37"/>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G61">
+    <sortCondition ref="B2:B61"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
@@ -24058,108 +24429,121 @@
     <hyperlink ref="D14" r:id="rId26" xr:uid="{00000000-0004-0000-0700-000019000000}"/>
     <hyperlink ref="A15" r:id="rId27" xr:uid="{00000000-0004-0000-0700-00001A000000}"/>
     <hyperlink ref="D15" r:id="rId28" xr:uid="{00000000-0004-0000-0700-00001B000000}"/>
-    <hyperlink ref="A16" r:id="rId29" xr:uid="{00000000-0004-0000-0700-00001C000000}"/>
-    <hyperlink ref="D16" r:id="rId30" xr:uid="{00000000-0004-0000-0700-00001D000000}"/>
-    <hyperlink ref="A17" r:id="rId31" xr:uid="{00000000-0004-0000-0700-00001E000000}"/>
-    <hyperlink ref="D17" r:id="rId32" xr:uid="{00000000-0004-0000-0700-00001F000000}"/>
-    <hyperlink ref="A18" r:id="rId33" xr:uid="{00000000-0004-0000-0700-000020000000}"/>
-    <hyperlink ref="D18" r:id="rId34" xr:uid="{00000000-0004-0000-0700-000021000000}"/>
-    <hyperlink ref="A19" r:id="rId35" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
-    <hyperlink ref="D19" r:id="rId36" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
-    <hyperlink ref="A20" r:id="rId37" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
-    <hyperlink ref="D20" r:id="rId38" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
-    <hyperlink ref="A21" r:id="rId39" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
-    <hyperlink ref="D21" r:id="rId40" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
-    <hyperlink ref="A22" r:id="rId41" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
-    <hyperlink ref="A23" r:id="rId42" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
-    <hyperlink ref="D23" r:id="rId43" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
-    <hyperlink ref="A24" r:id="rId44" xr:uid="{00000000-0004-0000-0700-00002B000000}"/>
-    <hyperlink ref="D24" r:id="rId45" xr:uid="{00000000-0004-0000-0700-00002C000000}"/>
-    <hyperlink ref="A25" r:id="rId46" xr:uid="{00000000-0004-0000-0700-00002D000000}"/>
-    <hyperlink ref="D25" r:id="rId47" xr:uid="{00000000-0004-0000-0700-00002E000000}"/>
-    <hyperlink ref="A26" r:id="rId48" xr:uid="{00000000-0004-0000-0700-00002F000000}"/>
-    <hyperlink ref="D26" r:id="rId49" xr:uid="{00000000-0004-0000-0700-000030000000}"/>
-    <hyperlink ref="A27" r:id="rId50" xr:uid="{00000000-0004-0000-0700-000031000000}"/>
-    <hyperlink ref="D27" r:id="rId51" xr:uid="{00000000-0004-0000-0700-000032000000}"/>
-    <hyperlink ref="A28" r:id="rId52" xr:uid="{00000000-0004-0000-0700-000033000000}"/>
-    <hyperlink ref="D28" r:id="rId53" xr:uid="{00000000-0004-0000-0700-000034000000}"/>
-    <hyperlink ref="A29" r:id="rId54" xr:uid="{00000000-0004-0000-0700-000035000000}"/>
-    <hyperlink ref="D29" r:id="rId55" xr:uid="{00000000-0004-0000-0700-000036000000}"/>
-    <hyperlink ref="A30" r:id="rId56" xr:uid="{00000000-0004-0000-0700-000037000000}"/>
-    <hyperlink ref="D30" r:id="rId57" xr:uid="{00000000-0004-0000-0700-000038000000}"/>
-    <hyperlink ref="A31" r:id="rId58" xr:uid="{00000000-0004-0000-0700-000039000000}"/>
-    <hyperlink ref="D31" r:id="rId59" xr:uid="{00000000-0004-0000-0700-00003A000000}"/>
-    <hyperlink ref="A32" r:id="rId60" xr:uid="{00000000-0004-0000-0700-00003B000000}"/>
-    <hyperlink ref="A33" r:id="rId61" xr:uid="{00000000-0004-0000-0700-00003C000000}"/>
-    <hyperlink ref="D33" r:id="rId62" xr:uid="{00000000-0004-0000-0700-00003D000000}"/>
-    <hyperlink ref="A34" r:id="rId63" xr:uid="{00000000-0004-0000-0700-00003E000000}"/>
-    <hyperlink ref="D34" r:id="rId64" xr:uid="{00000000-0004-0000-0700-00003F000000}"/>
-    <hyperlink ref="A35" r:id="rId65" xr:uid="{00000000-0004-0000-0700-000040000000}"/>
-    <hyperlink ref="D35" r:id="rId66" xr:uid="{00000000-0004-0000-0700-000041000000}"/>
-    <hyperlink ref="A36" r:id="rId67" xr:uid="{00000000-0004-0000-0700-000042000000}"/>
-    <hyperlink ref="D36" r:id="rId68" xr:uid="{00000000-0004-0000-0700-000043000000}"/>
-    <hyperlink ref="A37" r:id="rId69" xr:uid="{00000000-0004-0000-0700-000044000000}"/>
-    <hyperlink ref="A38" r:id="rId70" xr:uid="{00000000-0004-0000-0700-000045000000}"/>
-    <hyperlink ref="D38" r:id="rId71" xr:uid="{00000000-0004-0000-0700-000046000000}"/>
-    <hyperlink ref="A39" r:id="rId72" xr:uid="{00000000-0004-0000-0700-000047000000}"/>
-    <hyperlink ref="A40" r:id="rId73" xr:uid="{00000000-0004-0000-0700-000048000000}"/>
-    <hyperlink ref="D40" r:id="rId74" xr:uid="{00000000-0004-0000-0700-000049000000}"/>
-    <hyperlink ref="A41" r:id="rId75" xr:uid="{00000000-0004-0000-0700-00004A000000}"/>
-    <hyperlink ref="D41" r:id="rId76" xr:uid="{00000000-0004-0000-0700-00004B000000}"/>
-    <hyperlink ref="A42" r:id="rId77" xr:uid="{00000000-0004-0000-0700-00004C000000}"/>
-    <hyperlink ref="D42" r:id="rId78" xr:uid="{00000000-0004-0000-0700-00004D000000}"/>
-    <hyperlink ref="A43" r:id="rId79" xr:uid="{00000000-0004-0000-0700-00004E000000}"/>
-    <hyperlink ref="D43" r:id="rId80" xr:uid="{00000000-0004-0000-0700-00004F000000}"/>
-    <hyperlink ref="A44" r:id="rId81" xr:uid="{00000000-0004-0000-0700-000050000000}"/>
-    <hyperlink ref="A45" r:id="rId82" xr:uid="{00000000-0004-0000-0700-000051000000}"/>
-    <hyperlink ref="D45" r:id="rId83" xr:uid="{00000000-0004-0000-0700-000052000000}"/>
-    <hyperlink ref="A46" r:id="rId84" xr:uid="{00000000-0004-0000-0700-000053000000}"/>
-    <hyperlink ref="D46" r:id="rId85" xr:uid="{00000000-0004-0000-0700-000054000000}"/>
-    <hyperlink ref="A47" r:id="rId86" xr:uid="{00000000-0004-0000-0700-000055000000}"/>
-    <hyperlink ref="A48" r:id="rId87" xr:uid="{00000000-0004-0000-0700-000056000000}"/>
-    <hyperlink ref="D48" r:id="rId88" xr:uid="{00000000-0004-0000-0700-000057000000}"/>
-    <hyperlink ref="A49" r:id="rId89" xr:uid="{00000000-0004-0000-0700-000058000000}"/>
-    <hyperlink ref="D49" r:id="rId90" xr:uid="{00000000-0004-0000-0700-000059000000}"/>
+    <hyperlink ref="A17" r:id="rId29" xr:uid="{00000000-0004-0000-0700-00001C000000}"/>
+    <hyperlink ref="D17" r:id="rId30" xr:uid="{00000000-0004-0000-0700-00001D000000}"/>
+    <hyperlink ref="A18" r:id="rId31" xr:uid="{00000000-0004-0000-0700-00001E000000}"/>
+    <hyperlink ref="D18" r:id="rId32" xr:uid="{00000000-0004-0000-0700-00001F000000}"/>
+    <hyperlink ref="A20" r:id="rId33" xr:uid="{00000000-0004-0000-0700-000020000000}"/>
+    <hyperlink ref="D20" r:id="rId34" xr:uid="{00000000-0004-0000-0700-000021000000}"/>
+    <hyperlink ref="A21" r:id="rId35" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
+    <hyperlink ref="D21" r:id="rId36" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
+    <hyperlink ref="A22" r:id="rId37" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
+    <hyperlink ref="D22" r:id="rId38" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
+    <hyperlink ref="A23" r:id="rId39" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
+    <hyperlink ref="D23" r:id="rId40" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
+    <hyperlink ref="A25" r:id="rId41" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
+    <hyperlink ref="A26" r:id="rId42" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
+    <hyperlink ref="D26" r:id="rId43" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
+    <hyperlink ref="A27" r:id="rId44" xr:uid="{00000000-0004-0000-0700-00002B000000}"/>
+    <hyperlink ref="D27" r:id="rId45" xr:uid="{00000000-0004-0000-0700-00002C000000}"/>
+    <hyperlink ref="A28" r:id="rId46" xr:uid="{00000000-0004-0000-0700-00002D000000}"/>
+    <hyperlink ref="D28" r:id="rId47" xr:uid="{00000000-0004-0000-0700-00002E000000}"/>
+    <hyperlink ref="A29" r:id="rId48" xr:uid="{00000000-0004-0000-0700-00002F000000}"/>
+    <hyperlink ref="D29" r:id="rId49" xr:uid="{00000000-0004-0000-0700-000030000000}"/>
+    <hyperlink ref="A31" r:id="rId50" xr:uid="{00000000-0004-0000-0700-000031000000}"/>
+    <hyperlink ref="D31" r:id="rId51" xr:uid="{00000000-0004-0000-0700-000032000000}"/>
+    <hyperlink ref="A32" r:id="rId52" xr:uid="{00000000-0004-0000-0700-000033000000}"/>
+    <hyperlink ref="D32" r:id="rId53" xr:uid="{00000000-0004-0000-0700-000034000000}"/>
+    <hyperlink ref="A33" r:id="rId54" xr:uid="{00000000-0004-0000-0700-000035000000}"/>
+    <hyperlink ref="D33" r:id="rId55" xr:uid="{00000000-0004-0000-0700-000036000000}"/>
+    <hyperlink ref="A34" r:id="rId56" xr:uid="{00000000-0004-0000-0700-000037000000}"/>
+    <hyperlink ref="D34" r:id="rId57" xr:uid="{00000000-0004-0000-0700-000038000000}"/>
+    <hyperlink ref="A35" r:id="rId58" xr:uid="{00000000-0004-0000-0700-000039000000}"/>
+    <hyperlink ref="D35" r:id="rId59" xr:uid="{00000000-0004-0000-0700-00003A000000}"/>
+    <hyperlink ref="A36" r:id="rId60" xr:uid="{00000000-0004-0000-0700-00003B000000}"/>
+    <hyperlink ref="A37" r:id="rId61" xr:uid="{00000000-0004-0000-0700-00003C000000}"/>
+    <hyperlink ref="D37" r:id="rId62" xr:uid="{00000000-0004-0000-0700-00003D000000}"/>
+    <hyperlink ref="A38" r:id="rId63" xr:uid="{00000000-0004-0000-0700-00003E000000}"/>
+    <hyperlink ref="D38" r:id="rId64" xr:uid="{00000000-0004-0000-0700-00003F000000}"/>
+    <hyperlink ref="A39" r:id="rId65" xr:uid="{00000000-0004-0000-0700-000040000000}"/>
+    <hyperlink ref="D39" r:id="rId66" xr:uid="{00000000-0004-0000-0700-000041000000}"/>
+    <hyperlink ref="A40" r:id="rId67" xr:uid="{00000000-0004-0000-0700-000042000000}"/>
+    <hyperlink ref="D40" r:id="rId68" xr:uid="{00000000-0004-0000-0700-000043000000}"/>
+    <hyperlink ref="A41" r:id="rId69" xr:uid="{00000000-0004-0000-0700-000044000000}"/>
+    <hyperlink ref="A42" r:id="rId70" xr:uid="{00000000-0004-0000-0700-000045000000}"/>
+    <hyperlink ref="D42" r:id="rId71" xr:uid="{00000000-0004-0000-0700-000046000000}"/>
+    <hyperlink ref="A44" r:id="rId72" xr:uid="{00000000-0004-0000-0700-000047000000}"/>
+    <hyperlink ref="A45" r:id="rId73" xr:uid="{00000000-0004-0000-0700-000048000000}"/>
+    <hyperlink ref="D45" r:id="rId74" xr:uid="{00000000-0004-0000-0700-000049000000}"/>
+    <hyperlink ref="A46" r:id="rId75" xr:uid="{00000000-0004-0000-0700-00004A000000}"/>
+    <hyperlink ref="D46" r:id="rId76" xr:uid="{00000000-0004-0000-0700-00004B000000}"/>
+    <hyperlink ref="A47" r:id="rId77" xr:uid="{00000000-0004-0000-0700-00004C000000}"/>
+    <hyperlink ref="D47" r:id="rId78" xr:uid="{00000000-0004-0000-0700-00004D000000}"/>
+    <hyperlink ref="A48" r:id="rId79" xr:uid="{00000000-0004-0000-0700-00004E000000}"/>
+    <hyperlink ref="D48" r:id="rId80" xr:uid="{00000000-0004-0000-0700-00004F000000}"/>
+    <hyperlink ref="A49" r:id="rId81" xr:uid="{00000000-0004-0000-0700-000050000000}"/>
+    <hyperlink ref="A51" r:id="rId82" xr:uid="{00000000-0004-0000-0700-000051000000}"/>
+    <hyperlink ref="D51" r:id="rId83" xr:uid="{00000000-0004-0000-0700-000052000000}"/>
+    <hyperlink ref="A52" r:id="rId84" xr:uid="{00000000-0004-0000-0700-000053000000}"/>
+    <hyperlink ref="D52" r:id="rId85" xr:uid="{00000000-0004-0000-0700-000054000000}"/>
+    <hyperlink ref="A53" r:id="rId86" xr:uid="{00000000-0004-0000-0700-000055000000}"/>
+    <hyperlink ref="A54" r:id="rId87" xr:uid="{00000000-0004-0000-0700-000056000000}"/>
+    <hyperlink ref="D54" r:id="rId88" xr:uid="{00000000-0004-0000-0700-000057000000}"/>
+    <hyperlink ref="A55" r:id="rId89" xr:uid="{00000000-0004-0000-0700-000058000000}"/>
+    <hyperlink ref="D55" r:id="rId90" xr:uid="{00000000-0004-0000-0700-000059000000}"/>
     <hyperlink ref="F4" r:id="rId91" xr:uid="{DF403FE6-1627-4F46-AA11-F96FC9980006}"/>
-    <hyperlink ref="F5" r:id="rId92" xr:uid="{B78F4A8E-EE74-458F-8347-671E436E8F3C}"/>
-    <hyperlink ref="F9" r:id="rId93" xr:uid="{39517324-523C-4412-8BB3-40B5DFECE840}"/>
-    <hyperlink ref="F8" r:id="rId94" xr:uid="{B124E3A4-DC98-4342-AD08-8537B63C367C}"/>
-    <hyperlink ref="F6" r:id="rId95" xr:uid="{422D2254-90E9-4983-8AB2-9B9D84299FEE}"/>
-    <hyperlink ref="F12" r:id="rId96" xr:uid="{A5CAD0E0-9E6F-404F-8AF6-04181D1A6D53}"/>
-    <hyperlink ref="F16" r:id="rId97" xr:uid="{726F981B-C8C3-43D9-BBAF-F2B63EE92466}"/>
-    <hyperlink ref="F18" r:id="rId98" xr:uid="{FCD99014-ABE5-418D-97D0-F95F318DD886}"/>
-    <hyperlink ref="F20" r:id="rId99" xr:uid="{03F59C9B-11AB-4479-AA4D-20907F297E3B}"/>
-    <hyperlink ref="F15" r:id="rId100" xr:uid="{E4EEFAD8-5F84-48E0-A9F5-A7690E7ADC44}"/>
-    <hyperlink ref="F23" r:id="rId101" xr:uid="{B3DDA8FD-AFD3-4781-B298-DD6F56DC111C}"/>
-    <hyperlink ref="F45" r:id="rId102" xr:uid="{789F82DC-0665-484E-B374-AE9DE0A0AA79}"/>
-    <hyperlink ref="F41" r:id="rId103" xr:uid="{63BB88C7-27D2-441F-8E3A-797F8EC31475}"/>
-    <hyperlink ref="F42" r:id="rId104" xr:uid="{228A4998-A22D-4FB3-AED7-19B681CC3F64}"/>
-    <hyperlink ref="F43" r:id="rId105" xr:uid="{94EDB1D3-A6FE-4366-A54B-2B3D99711DF1}"/>
-    <hyperlink ref="F44" r:id="rId106" xr:uid="{87D4D722-670D-4B47-A5EF-0493F324D823}"/>
-    <hyperlink ref="F39" r:id="rId107" xr:uid="{B0EDF03B-0F41-4E94-B554-0ACA6FF9621F}"/>
-    <hyperlink ref="F38" r:id="rId108" xr:uid="{F456585B-C8D4-4402-89D0-58B088F52119}"/>
-    <hyperlink ref="F14" r:id="rId109" xr:uid="{E212C8F7-6274-412B-A6FC-6F6B56B365A5}"/>
-    <hyperlink ref="F47" r:id="rId110" xr:uid="{0D1856A5-DD5C-4BC0-ABB1-114A3A1CAD84}"/>
-    <hyperlink ref="F46" r:id="rId111" xr:uid="{4D85AEC2-BE95-4750-8965-284DB6E7C2DE}"/>
-    <hyperlink ref="F17" r:id="rId112" xr:uid="{4A04BB8E-6A94-45CE-9A07-6FBAAF68E8F7}"/>
-    <hyperlink ref="F25" r:id="rId113" xr:uid="{87E47286-E94D-4516-B9CC-3F6C8AA6877D}"/>
-    <hyperlink ref="F27" r:id="rId114" xr:uid="{143D2563-CE74-4253-87E6-C38FA3930AAE}"/>
-    <hyperlink ref="F28" r:id="rId115" xr:uid="{23A7D343-EF31-4679-B467-85F658530E40}"/>
-    <hyperlink ref="F29" r:id="rId116" xr:uid="{03E54634-433B-4C01-BDD7-902837B49DB7}"/>
-    <hyperlink ref="F31" r:id="rId117" xr:uid="{25498FDD-15AA-41B5-9A49-9F0C3844864C}"/>
-    <hyperlink ref="F32" r:id="rId118" xr:uid="{34F7E35A-CDB3-4111-A7A3-F0C4F594BAB2}"/>
-    <hyperlink ref="F34" r:id="rId119" xr:uid="{07DFBCA7-3328-483B-955D-376A2996BF06}"/>
-    <hyperlink ref="F35" r:id="rId120" xr:uid="{C98CD025-F14D-4363-9FC3-28730B20E84C}"/>
-    <hyperlink ref="F36" r:id="rId121" xr:uid="{D3D3CE1B-2999-498A-AE50-0BB1051AF1B2}"/>
-    <hyperlink ref="F11" r:id="rId122" xr:uid="{221C6E4B-7A04-40C5-A3CD-C748188A8641}"/>
-    <hyperlink ref="F22" r:id="rId123" xr:uid="{AB4AAE11-19D2-46FB-A8BE-6A3184FC5B02}"/>
-    <hyperlink ref="F24" r:id="rId124" xr:uid="{DE40F15B-4577-4E7F-9812-B2B5D4D03363}"/>
-    <hyperlink ref="F26" r:id="rId125" xr:uid="{9C0C1FF3-1C33-4479-980F-F5E40BE6B604}"/>
-    <hyperlink ref="F30" r:id="rId126" xr:uid="{363EAD84-CE15-45C4-B282-BFC1A250DFC2}"/>
-    <hyperlink ref="F33" r:id="rId127" xr:uid="{38256328-2691-4320-88AE-0D7AD5D1713B}"/>
-    <hyperlink ref="F21" r:id="rId128" xr:uid="{BE4C7A75-E144-4BB2-85B3-5563668D93FB}"/>
+    <hyperlink ref="F9" r:id="rId92" xr:uid="{39517324-523C-4412-8BB3-40B5DFECE840}"/>
+    <hyperlink ref="F8" r:id="rId93" xr:uid="{B124E3A4-DC98-4342-AD08-8537B63C367C}"/>
+    <hyperlink ref="F12" r:id="rId94" xr:uid="{A5CAD0E0-9E6F-404F-8AF6-04181D1A6D53}"/>
+    <hyperlink ref="F17" r:id="rId95" xr:uid="{726F981B-C8C3-43D9-BBAF-F2B63EE92466}"/>
+    <hyperlink ref="F20" r:id="rId96" xr:uid="{FCD99014-ABE5-418D-97D0-F95F318DD886}"/>
+    <hyperlink ref="F22" r:id="rId97" xr:uid="{03F59C9B-11AB-4479-AA4D-20907F297E3B}"/>
+    <hyperlink ref="F15" r:id="rId98" xr:uid="{E4EEFAD8-5F84-48E0-A9F5-A7690E7ADC44}"/>
+    <hyperlink ref="F26" r:id="rId99" xr:uid="{B3DDA8FD-AFD3-4781-B298-DD6F56DC111C}"/>
+    <hyperlink ref="F51" r:id="rId100" xr:uid="{789F82DC-0665-484E-B374-AE9DE0A0AA79}"/>
+    <hyperlink ref="F46" r:id="rId101" xr:uid="{63BB88C7-27D2-441F-8E3A-797F8EC31475}"/>
+    <hyperlink ref="F47" r:id="rId102" xr:uid="{228A4998-A22D-4FB3-AED7-19B681CC3F64}"/>
+    <hyperlink ref="F48" r:id="rId103" xr:uid="{94EDB1D3-A6FE-4366-A54B-2B3D99711DF1}"/>
+    <hyperlink ref="F49" r:id="rId104" xr:uid="{87D4D722-670D-4B47-A5EF-0493F324D823}"/>
+    <hyperlink ref="F44" r:id="rId105" xr:uid="{B0EDF03B-0F41-4E94-B554-0ACA6FF9621F}"/>
+    <hyperlink ref="F42" r:id="rId106" xr:uid="{F456585B-C8D4-4402-89D0-58B088F52119}"/>
+    <hyperlink ref="F14" r:id="rId107" xr:uid="{E212C8F7-6274-412B-A6FC-6F6B56B365A5}"/>
+    <hyperlink ref="F53" r:id="rId108" xr:uid="{0D1856A5-DD5C-4BC0-ABB1-114A3A1CAD84}"/>
+    <hyperlink ref="F52" r:id="rId109" xr:uid="{4D85AEC2-BE95-4750-8965-284DB6E7C2DE}"/>
+    <hyperlink ref="F18" r:id="rId110" xr:uid="{4A04BB8E-6A94-45CE-9A07-6FBAAF68E8F7}"/>
+    <hyperlink ref="F28" r:id="rId111" xr:uid="{87E47286-E94D-4516-B9CC-3F6C8AA6877D}"/>
+    <hyperlink ref="F31" r:id="rId112" xr:uid="{143D2563-CE74-4253-87E6-C38FA3930AAE}"/>
+    <hyperlink ref="F32" r:id="rId113" xr:uid="{23A7D343-EF31-4679-B467-85F658530E40}"/>
+    <hyperlink ref="F33" r:id="rId114" xr:uid="{03E54634-433B-4C01-BDD7-902837B49DB7}"/>
+    <hyperlink ref="F35" r:id="rId115" xr:uid="{25498FDD-15AA-41B5-9A49-9F0C3844864C}"/>
+    <hyperlink ref="F36" r:id="rId116" xr:uid="{34F7E35A-CDB3-4111-A7A3-F0C4F594BAB2}"/>
+    <hyperlink ref="F38" r:id="rId117" xr:uid="{07DFBCA7-3328-483B-955D-376A2996BF06}"/>
+    <hyperlink ref="F39" r:id="rId118" xr:uid="{C98CD025-F14D-4363-9FC3-28730B20E84C}"/>
+    <hyperlink ref="F40" r:id="rId119" xr:uid="{D3D3CE1B-2999-498A-AE50-0BB1051AF1B2}"/>
+    <hyperlink ref="F11" r:id="rId120" xr:uid="{221C6E4B-7A04-40C5-A3CD-C748188A8641}"/>
+    <hyperlink ref="F25" r:id="rId121" xr:uid="{AB4AAE11-19D2-46FB-A8BE-6A3184FC5B02}"/>
+    <hyperlink ref="F27" r:id="rId122" xr:uid="{DE40F15B-4577-4E7F-9812-B2B5D4D03363}"/>
+    <hyperlink ref="F29" r:id="rId123" xr:uid="{9C0C1FF3-1C33-4479-980F-F5E40BE6B604}"/>
+    <hyperlink ref="F34" r:id="rId124" xr:uid="{363EAD84-CE15-45C4-B282-BFC1A250DFC2}"/>
+    <hyperlink ref="F37" r:id="rId125" xr:uid="{38256328-2691-4320-88AE-0D7AD5D1713B}"/>
+    <hyperlink ref="F23" r:id="rId126" xr:uid="{BE4C7A75-E144-4BB2-85B3-5563668D93FB}"/>
+    <hyperlink ref="F5" r:id="rId127" xr:uid="{22EBF509-75C8-4B35-8E73-997AB43A9A0E}"/>
+    <hyperlink ref="F6" r:id="rId128" xr:uid="{74342603-D18F-4AC3-AF38-677E4CD417B5}"/>
+    <hyperlink ref="F2" r:id="rId129" xr:uid="{A0BE881F-A776-4D43-9393-9B6FCDE5249A}"/>
+    <hyperlink ref="F3" r:id="rId130" xr:uid="{6B6F9A54-C7A4-448D-9B2C-F7E65DD60B62}"/>
+    <hyperlink ref="D19" r:id="rId131" xr:uid="{D11EAD54-EC8A-419C-9C6D-6CA420112945}"/>
+    <hyperlink ref="D50" r:id="rId132" xr:uid="{E96D0253-571D-4116-8E31-AD5D5A733472}"/>
+    <hyperlink ref="D16" r:id="rId133" xr:uid="{665BE8A1-639D-44FF-9F53-2F70D0B52033}"/>
+    <hyperlink ref="D43" r:id="rId134" xr:uid="{6E73B62C-F1F1-4C27-964C-4D523B61D8BB}"/>
+    <hyperlink ref="A19" r:id="rId135" xr:uid="{7AED9D98-563D-4E85-B93D-FBE33D266A0E}"/>
+    <hyperlink ref="A16" r:id="rId136" xr:uid="{09C25B74-3734-4D1A-B9AD-B58BB3EB2C53}"/>
+    <hyperlink ref="A24" r:id="rId137" xr:uid="{794E26A9-D6A2-4665-B2C5-FC8C8A797A1D}"/>
+    <hyperlink ref="A43" r:id="rId138" xr:uid="{4451BFF2-BC59-42D5-85D7-97B19DAE0C3D}"/>
+    <hyperlink ref="A50" r:id="rId139" xr:uid="{E221A161-8AF4-40B3-9E43-019C00D65D95}"/>
+    <hyperlink ref="D30" r:id="rId140" xr:uid="{D9275C9F-A502-484C-9C5C-36DC78E8AC35}"/>
+    <hyperlink ref="F30" r:id="rId141" xr:uid="{33FEB22A-5DE4-49D3-B6EC-E9397F7A8393}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId142"/>
 </worksheet>
 </file>
</xml_diff>